<commit_message>
added test for RKI H
</commit_message>
<xml_diff>
--- a/data/20200511_Nowcasting_Zahlen.xlsx
+++ b/data/20200511_Nowcasting_Zahlen.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10509"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\software_hardware\COVID-19\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/la5373/Documents/Code/Julia/ReproductionNumbers/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA34B102-3A5F-8440-946F-CD29A8E5FCD8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21943" windowHeight="7200" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15100" windowHeight="25600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Nowcast_R" sheetId="1" r:id="rId1"/>
@@ -17,12 +18,12 @@
     <sheet name="MW + STD Schätzer" sheetId="4" r:id="rId3"/>
     <sheet name="Erläuterungen" sheetId="5" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="181029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="124">
   <si>
     <t>Untere Grenze des 95%-Prädiktionsintervalls der Anzahl Neuerkrankungen</t>
   </si>
@@ -69,27 +70,6 @@
     <t>R(NEU-A)</t>
   </si>
   <si>
-    <t>Montag</t>
-  </si>
-  <si>
-    <t>Dienstag</t>
-  </si>
-  <si>
-    <t>Mittwoch</t>
-  </si>
-  <si>
-    <t>Donnerstag</t>
-  </si>
-  <si>
-    <t>Freitag</t>
-  </si>
-  <si>
-    <t>Samstag</t>
-  </si>
-  <si>
-    <t>Sonntag</t>
-  </si>
-  <si>
     <t>Erkrankung</t>
   </si>
   <si>
@@ -412,13 +392,16 @@
   </si>
   <si>
     <t>MAE(RKI-H vs. NEU-HA)</t>
+  </si>
+  <si>
+    <t>Wochentag für RKI Tagesbericht</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
@@ -604,9 +587,9 @@
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
-    <cellStyle name="Standard 2" xfId="1"/>
-    <cellStyle name="Standard 3" xfId="2"/>
-    <cellStyle name="Standard 4" xfId="3"/>
+    <cellStyle name="Standard 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Standard 3" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="Standard 4" xfId="3" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -702,6 +685,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -737,6 +737,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -912,51 +929,51 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AJ152"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="R50" activePane="bottomRight" state="frozenSplit"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="N21" activePane="bottomRight" state="frozenSplit"/>
       <selection activeCell="J11" sqref="H9:J11"/>
       <selection pane="topRight" activeCell="K1" sqref="K1"/>
       <selection pane="bottomLeft" activeCell="A12" sqref="A12"/>
-      <selection pane="bottomRight" activeCell="AB9" sqref="AB9"/>
+      <selection pane="bottomRight" activeCell="AL95" sqref="A95:AL116"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.15234375" defaultRowHeight="14.6"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="17" style="12" customWidth="1"/>
     <col min="2" max="2" width="17" style="14" customWidth="1"/>
-    <col min="3" max="3" width="15.69140625" style="12" customWidth="1"/>
-    <col min="4" max="9" width="9.15234375" style="12"/>
-    <col min="10" max="10" width="9.15234375" style="24"/>
-    <col min="11" max="11" width="9.15234375" style="12"/>
-    <col min="12" max="12" width="15.53515625" style="12" customWidth="1"/>
-    <col min="13" max="14" width="9.15234375" style="12"/>
-    <col min="15" max="15" width="9.15234375" style="17"/>
-    <col min="16" max="16" width="11.921875" style="15" customWidth="1"/>
-    <col min="17" max="17" width="15.69140625" style="12" customWidth="1"/>
-    <col min="18" max="18" width="12.53515625" style="14" customWidth="1"/>
-    <col min="19" max="19" width="9.15234375" style="17"/>
-    <col min="20" max="20" width="10.69140625" style="14" customWidth="1"/>
-    <col min="21" max="21" width="9.15234375" style="18"/>
-    <col min="22" max="22" width="10.84375" style="14" customWidth="1"/>
-    <col min="23" max="23" width="11.53515625" style="18" customWidth="1"/>
-    <col min="24" max="24" width="12.84375" style="14" customWidth="1"/>
-    <col min="25" max="25" width="9.15234375" style="18"/>
-    <col min="26" max="26" width="9.15234375" style="12"/>
-    <col min="27" max="27" width="9.15234375" style="17"/>
-    <col min="28" max="29" width="9.15234375" style="12"/>
-    <col min="30" max="31" width="9.15234375" style="17"/>
-    <col min="32" max="16384" width="9.15234375" style="12"/>
+    <col min="3" max="3" width="15.6640625" style="12" customWidth="1"/>
+    <col min="4" max="9" width="9.1640625" style="12"/>
+    <col min="10" max="10" width="9.1640625" style="24"/>
+    <col min="11" max="11" width="9.1640625" style="12"/>
+    <col min="12" max="12" width="15.5" style="12" customWidth="1"/>
+    <col min="13" max="14" width="9.1640625" style="12"/>
+    <col min="15" max="15" width="9.1640625" style="17"/>
+    <col min="16" max="16" width="12" style="15" customWidth="1"/>
+    <col min="17" max="17" width="15.6640625" style="12" customWidth="1"/>
+    <col min="18" max="18" width="12.5" style="14" customWidth="1"/>
+    <col min="19" max="19" width="9.1640625" style="17"/>
+    <col min="20" max="20" width="10.6640625" style="14" customWidth="1"/>
+    <col min="21" max="21" width="9.1640625" style="18"/>
+    <col min="22" max="22" width="10.83203125" style="14" customWidth="1"/>
+    <col min="23" max="23" width="11.5" style="18" customWidth="1"/>
+    <col min="24" max="24" width="12.83203125" style="14" customWidth="1"/>
+    <col min="25" max="25" width="9.1640625" style="18"/>
+    <col min="26" max="26" width="9.1640625" style="12"/>
+    <col min="27" max="27" width="9.1640625" style="17"/>
+    <col min="28" max="29" width="9.1640625" style="12"/>
+    <col min="30" max="31" width="9.1640625" style="17"/>
+    <col min="32" max="16384" width="9.1640625" style="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" s="19" customFormat="1" ht="160.30000000000001">
+    <row r="1" spans="1:36" s="19" customFormat="1" ht="160" x14ac:dyDescent="0.2">
       <c r="A1" s="19" t="s">
         <v>9</v>
       </c>
       <c r="B1" s="36" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="C1" s="19" t="s">
         <v>5</v>
@@ -965,10 +982,10 @@
         <v>10</v>
       </c>
       <c r="E1" s="19" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="F1" s="19" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="G1" s="20" t="s">
         <v>11</v>
@@ -989,43 +1006,43 @@
         <v>3</v>
       </c>
       <c r="M1" s="21" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="N1" s="21" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="O1" s="29" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="P1" s="22" t="s">
         <v>4</v>
       </c>
       <c r="Q1" s="19" t="s">
-        <v>5</v>
+        <v>123</v>
       </c>
       <c r="R1" s="21" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="S1" s="20" t="s">
         <v>7</v>
       </c>
       <c r="T1" s="20" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="U1" s="29" t="s">
         <v>8</v>
       </c>
       <c r="V1" s="20" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="W1" s="20" t="s">
         <v>12</v>
       </c>
       <c r="X1" s="20" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="Y1" s="20" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="Z1" s="20" t="s">
         <v>13</v>
@@ -1034,34 +1051,34 @@
         <v>14</v>
       </c>
       <c r="AB1" s="20" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="AC1" s="20" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="AD1" s="34" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="AE1" s="34" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="AF1" s="29" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="AG1" s="20" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="AH1" s="19" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="AI1" s="19" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="AJ1" s="19" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="2" spans="1:36">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A2" s="11">
         <v>43892</v>
       </c>
@@ -1115,7 +1132,7 @@
       <c r="AB2" s="39"/>
       <c r="AC2" s="39"/>
     </row>
-    <row r="3" spans="1:36">
+    <row r="3" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A3" s="11">
         <v>43893</v>
       </c>
@@ -1169,7 +1186,7 @@
       <c r="AB3" s="39"/>
       <c r="AC3" s="39"/>
     </row>
-    <row r="4" spans="1:36">
+    <row r="4" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A4" s="11">
         <v>43894</v>
       </c>
@@ -1223,7 +1240,7 @@
       <c r="AB4" s="39"/>
       <c r="AC4" s="39"/>
     </row>
-    <row r="5" spans="1:36">
+    <row r="5" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A5" s="11">
         <v>43895</v>
       </c>
@@ -1283,7 +1300,7 @@
       <c r="AB5" s="39"/>
       <c r="AC5" s="39"/>
     </row>
-    <row r="6" spans="1:36">
+    <row r="6" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A6" s="11">
         <v>43896</v>
       </c>
@@ -1351,7 +1368,7 @@
       <c r="AB6" s="39"/>
       <c r="AC6" s="39"/>
     </row>
-    <row r="7" spans="1:36">
+    <row r="7" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A7" s="11">
         <v>43897</v>
       </c>
@@ -1419,7 +1436,7 @@
       <c r="AB7" s="39"/>
       <c r="AC7" s="39"/>
     </row>
-    <row r="8" spans="1:36">
+    <row r="8" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A8" s="11">
         <v>43898</v>
       </c>
@@ -1487,7 +1504,7 @@
       <c r="AB8" s="39"/>
       <c r="AC8" s="39"/>
     </row>
-    <row r="9" spans="1:36" s="10" customFormat="1">
+    <row r="9" spans="1:36" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="3">
         <v>43899</v>
       </c>
@@ -1573,7 +1590,7 @@
       <c r="AD9" s="8"/>
       <c r="AE9" s="8"/>
     </row>
-    <row r="10" spans="1:36" s="10" customFormat="1">
+    <row r="10" spans="1:36" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="3">
         <v>43900</v>
       </c>
@@ -1659,7 +1676,7 @@
       <c r="AD10" s="8"/>
       <c r="AE10" s="8"/>
     </row>
-    <row r="11" spans="1:36" s="10" customFormat="1">
+    <row r="11" spans="1:36" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="3">
         <v>43901</v>
       </c>
@@ -1745,7 +1762,7 @@
       <c r="AD11" s="8"/>
       <c r="AE11" s="8"/>
     </row>
-    <row r="12" spans="1:36" s="10" customFormat="1">
+    <row r="12" spans="1:36" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12" s="3">
         <v>43902</v>
       </c>
@@ -1837,7 +1854,7 @@
       <c r="AD12" s="8"/>
       <c r="AE12" s="8"/>
     </row>
-    <row r="13" spans="1:36" s="10" customFormat="1">
+    <row r="13" spans="1:36" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="3">
         <v>43903</v>
       </c>
@@ -1935,7 +1952,7 @@
       <c r="AD13" s="8"/>
       <c r="AE13" s="8"/>
     </row>
-    <row r="14" spans="1:36" s="10" customFormat="1">
+    <row r="14" spans="1:36" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="3">
         <v>43904</v>
       </c>
@@ -2033,7 +2050,7 @@
       <c r="AD14" s="8"/>
       <c r="AE14" s="8"/>
     </row>
-    <row r="15" spans="1:36" s="10" customFormat="1">
+    <row r="15" spans="1:36" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="3">
         <v>43905</v>
       </c>
@@ -2143,7 +2160,7 @@
         <v>2125.656595947793</v>
       </c>
     </row>
-    <row r="16" spans="1:36">
+    <row r="16" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A16" s="11">
         <v>43906</v>
       </c>
@@ -2256,7 +2273,7 @@
         <v>1291.9747348990868</v>
       </c>
     </row>
-    <row r="17" spans="1:36">
+    <row r="17" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A17" s="11">
         <v>43907</v>
       </c>
@@ -2369,7 +2386,7 @@
         <v>1905.3647537779116</v>
       </c>
     </row>
-    <row r="18" spans="1:36">
+    <row r="18" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A18" s="11">
         <v>43908</v>
       </c>
@@ -2482,7 +2499,7 @@
         <v>1596.244338865451</v>
       </c>
     </row>
-    <row r="19" spans="1:36">
+    <row r="19" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A19" s="11">
         <v>43909</v>
       </c>
@@ -2595,7 +2612,7 @@
         <v>1777.888937465349</v>
       </c>
     </row>
-    <row r="20" spans="1:36">
+    <row r="20" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A20" s="11">
         <v>43910</v>
       </c>
@@ -2708,7 +2725,7 @@
         <v>781.68835229175511</v>
       </c>
     </row>
-    <row r="21" spans="1:36">
+    <row r="21" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A21" s="11">
         <v>43911</v>
       </c>
@@ -2821,7 +2838,7 @@
         <v>1189.1580175637691</v>
       </c>
     </row>
-    <row r="22" spans="1:36">
+    <row r="22" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A22" s="11">
         <v>43912</v>
       </c>
@@ -2934,7 +2951,7 @@
         <v>1275.6839173067347</v>
       </c>
     </row>
-    <row r="23" spans="1:36" s="10" customFormat="1">
+    <row r="23" spans="1:36" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A23" s="3">
         <v>43913</v>
       </c>
@@ -3050,7 +3067,7 @@
         <v>360.95701848413137</v>
       </c>
     </row>
-    <row r="24" spans="1:36" s="10" customFormat="1">
+    <row r="24" spans="1:36" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A24" s="3">
         <v>43914</v>
       </c>
@@ -3166,7 +3183,7 @@
         <v>289.67897577949407</v>
       </c>
     </row>
-    <row r="25" spans="1:36" s="10" customFormat="1">
+    <row r="25" spans="1:36" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A25" s="3">
         <v>43915</v>
       </c>
@@ -3282,7 +3299,7 @@
         <v>159.86410165614689</v>
       </c>
     </row>
-    <row r="26" spans="1:36" s="10" customFormat="1">
+    <row r="26" spans="1:36" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A26" s="3">
         <v>43916</v>
       </c>
@@ -3398,7 +3415,7 @@
         <v>125.6994767859178</v>
       </c>
     </row>
-    <row r="27" spans="1:36" s="10" customFormat="1">
+    <row r="27" spans="1:36" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A27" s="3">
         <v>43917</v>
       </c>
@@ -3514,7 +3531,7 @@
         <v>175.48387770739737</v>
       </c>
     </row>
-    <row r="28" spans="1:36" s="10" customFormat="1">
+    <row r="28" spans="1:36" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A28" s="3">
         <v>43918</v>
       </c>
@@ -3630,7 +3647,7 @@
         <v>12.501750424077727</v>
       </c>
     </row>
-    <row r="29" spans="1:36" s="10" customFormat="1">
+    <row r="29" spans="1:36" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A29" s="3">
         <v>43919</v>
       </c>
@@ -3746,7 +3763,7 @@
         <v>509.73310504616074</v>
       </c>
     </row>
-    <row r="30" spans="1:36">
+    <row r="30" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A30" s="11">
         <v>43920</v>
       </c>
@@ -3859,7 +3876,7 @@
         <v>601.12729525468285</v>
       </c>
     </row>
-    <row r="31" spans="1:36">
+    <row r="31" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A31" s="11">
         <v>43921</v>
       </c>
@@ -3972,7 +3989,7 @@
         <v>110.86334324796189</v>
       </c>
     </row>
-    <row r="32" spans="1:36">
+    <row r="32" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A32" s="11">
         <v>43922</v>
       </c>
@@ -4085,7 +4102,7 @@
         <v>339.25010748843988</v>
       </c>
     </row>
-    <row r="33" spans="1:36">
+    <row r="33" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A33" s="11">
         <v>43923</v>
       </c>
@@ -4198,7 +4215,7 @@
         <v>84.501159190053841</v>
       </c>
     </row>
-    <row r="34" spans="1:36">
+    <row r="34" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A34" s="11">
         <v>43924</v>
       </c>
@@ -4330,7 +4347,7 @@
         <v>92.284795121283423</v>
       </c>
     </row>
-    <row r="35" spans="1:36">
+    <row r="35" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A35" s="11">
         <v>43925</v>
       </c>
@@ -4462,7 +4479,7 @@
         <v>463.98248323987445</v>
       </c>
     </row>
-    <row r="36" spans="1:36">
+    <row r="36" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A36" s="11">
         <v>43926</v>
       </c>
@@ -4594,7 +4611,7 @@
         <v>650.18287772671374</v>
       </c>
     </row>
-    <row r="37" spans="1:36" s="10" customFormat="1">
+    <row r="37" spans="1:36" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A37" s="3">
         <v>43927</v>
       </c>
@@ -4726,7 +4743,7 @@
         <v>158.82084843891698</v>
       </c>
     </row>
-    <row r="38" spans="1:36" s="10" customFormat="1">
+    <row r="38" spans="1:36" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A38" s="3">
         <v>43928</v>
       </c>
@@ -4858,7 +4875,7 @@
         <v>11.365576931816122</v>
       </c>
     </row>
-    <row r="39" spans="1:36" s="10" customFormat="1">
+    <row r="39" spans="1:36" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A39" s="3">
         <v>43929</v>
       </c>
@@ -4990,7 +5007,7 @@
         <v>20.04779224030699</v>
       </c>
     </row>
-    <row r="40" spans="1:36" s="10" customFormat="1">
+    <row r="40" spans="1:36" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A40" s="3">
         <v>43930</v>
       </c>
@@ -5122,7 +5139,7 @@
         <v>36.8838634604258</v>
       </c>
     </row>
-    <row r="41" spans="1:36" s="10" customFormat="1">
+    <row r="41" spans="1:36" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A41" s="3">
         <v>43931</v>
       </c>
@@ -5254,7 +5271,7 @@
         <v>191.71069849973219</v>
       </c>
     </row>
-    <row r="42" spans="1:36" s="10" customFormat="1">
+    <row r="42" spans="1:36" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A42" s="3">
         <v>43932</v>
       </c>
@@ -5386,7 +5403,7 @@
         <v>300.55040226486653</v>
       </c>
     </row>
-    <row r="43" spans="1:36" s="10" customFormat="1">
+    <row r="43" spans="1:36" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A43" s="3">
         <v>43933</v>
       </c>
@@ -5518,7 +5535,7 @@
         <v>233.18184376051113</v>
       </c>
     </row>
-    <row r="44" spans="1:36">
+    <row r="44" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A44" s="11">
         <v>43934</v>
       </c>
@@ -5650,7 +5667,7 @@
         <v>66.014971198800822</v>
       </c>
     </row>
-    <row r="45" spans="1:36">
+    <row r="45" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A45" s="11">
         <v>43935</v>
       </c>
@@ -5782,7 +5799,7 @@
         <v>118.95462402912426</v>
       </c>
     </row>
-    <row r="46" spans="1:36">
+    <row r="46" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A46" s="11">
         <v>43936</v>
       </c>
@@ -5914,7 +5931,7 @@
         <v>166.64683100807702</v>
       </c>
     </row>
-    <row r="47" spans="1:36">
+    <row r="47" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A47" s="11">
         <v>43937</v>
       </c>
@@ -6046,7 +6063,7 @@
         <v>127.51085289406865</v>
       </c>
     </row>
-    <row r="48" spans="1:36">
+    <row r="48" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A48" s="11">
         <v>43938</v>
       </c>
@@ -6178,7 +6195,7 @@
         <v>70.704375162642464</v>
       </c>
     </row>
-    <row r="49" spans="1:36">
+    <row r="49" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A49" s="11">
         <v>43939</v>
       </c>
@@ -6310,7 +6327,7 @@
         <v>95.610368772189531</v>
       </c>
     </row>
-    <row r="50" spans="1:36">
+    <row r="50" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A50" s="11">
         <v>43940</v>
       </c>
@@ -6442,7 +6459,7 @@
         <v>152.43771155347167</v>
       </c>
     </row>
-    <row r="51" spans="1:36" s="10" customFormat="1">
+    <row r="51" spans="1:36" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A51" s="3">
         <v>43941</v>
       </c>
@@ -6574,7 +6591,7 @@
         <v>98.226527305305126</v>
       </c>
     </row>
-    <row r="52" spans="1:36" s="10" customFormat="1">
+    <row r="52" spans="1:36" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A52" s="3">
         <v>43942</v>
       </c>
@@ -6706,7 +6723,7 @@
         <v>5.266044095123334</v>
       </c>
     </row>
-    <row r="53" spans="1:36" s="10" customFormat="1">
+    <row r="53" spans="1:36" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A53" s="3">
         <v>43943</v>
       </c>
@@ -6838,7 +6855,7 @@
         <v>23.945396695415411</v>
       </c>
     </row>
-    <row r="54" spans="1:36" s="10" customFormat="1">
+    <row r="54" spans="1:36" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A54" s="3">
         <v>43944</v>
       </c>
@@ -6970,7 +6987,7 @@
         <v>47.444948843038674</v>
       </c>
     </row>
-    <row r="55" spans="1:36" s="10" customFormat="1">
+    <row r="55" spans="1:36" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A55" s="3">
         <v>43945</v>
       </c>
@@ -7102,7 +7119,7 @@
         <v>10.443312181678266</v>
       </c>
     </row>
-    <row r="56" spans="1:36" s="10" customFormat="1">
+    <row r="56" spans="1:36" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A56" s="3">
         <v>43946</v>
       </c>
@@ -7234,7 +7251,7 @@
         <v>95.206493871852444</v>
       </c>
     </row>
-    <row r="57" spans="1:36" s="10" customFormat="1">
+    <row r="57" spans="1:36" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A57" s="3">
         <v>43947</v>
       </c>
@@ -7366,7 +7383,7 @@
         <v>138.27504240383587</v>
       </c>
     </row>
-    <row r="58" spans="1:36">
+    <row r="58" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A58" s="11">
         <v>43948</v>
       </c>
@@ -7492,7 +7509,7 @@
         <v>107.45128558771523</v>
       </c>
     </row>
-    <row r="59" spans="1:36">
+    <row r="59" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A59" s="11">
         <v>43949</v>
       </c>
@@ -7618,7 +7635,7 @@
         <v>21.266750293881842</v>
       </c>
     </row>
-    <row r="60" spans="1:36">
+    <row r="60" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A60" s="11">
         <v>43950</v>
       </c>
@@ -7744,7 +7761,7 @@
         <v>2.1541625280333392</v>
       </c>
     </row>
-    <row r="61" spans="1:36">
+    <row r="61" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A61" s="11">
         <v>43951</v>
       </c>
@@ -7870,7 +7887,7 @@
         <v>46.654127504114172</v>
       </c>
     </row>
-    <row r="62" spans="1:36">
+    <row r="62" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A62" s="11">
         <v>43952</v>
       </c>
@@ -7996,7 +8013,7 @@
         <v>45.74159902183078</v>
       </c>
     </row>
-    <row r="63" spans="1:36">
+    <row r="63" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A63" s="11">
         <v>43953</v>
       </c>
@@ -8122,7 +8139,7 @@
         <v>22.87693741355065</v>
       </c>
     </row>
-    <row r="64" spans="1:36" s="10" customFormat="1">
+    <row r="64" spans="1:36" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A64" s="3">
         <v>43954</v>
       </c>
@@ -8248,7 +8265,7 @@
         <v>56.570442695835368</v>
       </c>
     </row>
-    <row r="65" spans="1:36" s="10" customFormat="1">
+    <row r="65" spans="1:36" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A65" s="3">
         <v>43955</v>
       </c>
@@ -8350,7 +8367,7 @@
       <c r="AI65" s="17"/>
       <c r="AJ65" s="17"/>
     </row>
-    <row r="66" spans="1:36" s="10" customFormat="1">
+    <row r="66" spans="1:36" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A66" s="3">
         <v>43956</v>
       </c>
@@ -8452,7 +8469,7 @@
       <c r="AI66" s="17"/>
       <c r="AJ66" s="17"/>
     </row>
-    <row r="67" spans="1:36" s="10" customFormat="1">
+    <row r="67" spans="1:36" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A67" s="3">
         <v>43957</v>
       </c>
@@ -8554,7 +8571,7 @@
       <c r="AI67" s="17"/>
       <c r="AJ67" s="17"/>
     </row>
-    <row r="68" spans="1:36">
+    <row r="68" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A68" s="23"/>
       <c r="B68" s="37"/>
       <c r="M68" s="14"/>
@@ -8566,7 +8583,7 @@
       <c r="AI68" s="17"/>
       <c r="AJ68" s="17"/>
     </row>
-    <row r="69" spans="1:36">
+    <row r="69" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A69" s="23"/>
       <c r="B69" s="38"/>
       <c r="M69" s="14"/>
@@ -8576,7 +8593,7 @@
       <c r="AI69" s="17"/>
       <c r="AJ69" s="17"/>
     </row>
-    <row r="70" spans="1:36">
+    <row r="70" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A70" s="23"/>
       <c r="B70" s="38"/>
       <c r="M70" s="14"/>
@@ -8586,7 +8603,7 @@
       <c r="AI70" s="17"/>
       <c r="AJ70" s="17"/>
     </row>
-    <row r="71" spans="1:36">
+    <row r="71" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A71" s="23"/>
       <c r="B71" s="38"/>
       <c r="M71" s="14"/>
@@ -8595,7 +8612,7 @@
       <c r="AI71" s="17"/>
       <c r="AJ71" s="17"/>
     </row>
-    <row r="72" spans="1:36">
+    <row r="72" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A72" s="23"/>
       <c r="B72" s="38"/>
       <c r="M72" s="14"/>
@@ -8604,330 +8621,229 @@
       <c r="AI72" s="17"/>
       <c r="AJ72" s="17"/>
     </row>
-    <row r="73" spans="1:36">
+    <row r="73" spans="1:36" x14ac:dyDescent="0.2">
       <c r="M73" s="14"/>
       <c r="N73" s="14"/>
       <c r="AH73" s="17"/>
       <c r="AI73" s="17"/>
       <c r="AJ73" s="17"/>
     </row>
-    <row r="74" spans="1:36">
+    <row r="74" spans="1:36" x14ac:dyDescent="0.2">
       <c r="M74" s="14"/>
       <c r="N74" s="14"/>
       <c r="AH74" s="17"/>
       <c r="AI74" s="17"/>
       <c r="AJ74" s="17"/>
     </row>
-    <row r="75" spans="1:36">
+    <row r="75" spans="1:36" x14ac:dyDescent="0.2">
       <c r="M75" s="14"/>
       <c r="N75" s="14"/>
       <c r="AH75" s="17"/>
       <c r="AI75" s="17"/>
       <c r="AJ75" s="17"/>
     </row>
-    <row r="76" spans="1:36">
+    <row r="76" spans="1:36" x14ac:dyDescent="0.2">
       <c r="M76" s="14"/>
       <c r="N76" s="14"/>
       <c r="AH76" s="17"/>
       <c r="AI76" s="17"/>
       <c r="AJ76" s="17"/>
     </row>
-    <row r="77" spans="1:36">
+    <row r="77" spans="1:36" x14ac:dyDescent="0.2">
       <c r="M77" s="14"/>
       <c r="N77" s="14"/>
       <c r="AH77" s="17"/>
       <c r="AI77" s="17"/>
       <c r="AJ77" s="17"/>
     </row>
-    <row r="78" spans="1:36">
+    <row r="78" spans="1:36" x14ac:dyDescent="0.2">
       <c r="M78" s="14"/>
       <c r="N78" s="14"/>
       <c r="AH78" s="17"/>
       <c r="AI78" s="17"/>
       <c r="AJ78" s="17"/>
     </row>
-    <row r="79" spans="1:36">
+    <row r="79" spans="1:36" x14ac:dyDescent="0.2">
       <c r="M79" s="14"/>
       <c r="N79" s="14"/>
       <c r="AH79" s="17"/>
       <c r="AI79" s="17"/>
       <c r="AJ79" s="17"/>
     </row>
-    <row r="80" spans="1:36">
+    <row r="80" spans="1:36" x14ac:dyDescent="0.2">
       <c r="M80" s="14"/>
       <c r="N80" s="14"/>
       <c r="AH80" s="17"/>
       <c r="AI80" s="17"/>
       <c r="AJ80" s="17"/>
     </row>
-    <row r="81" spans="13:36">
+    <row r="81" spans="13:36" x14ac:dyDescent="0.2">
       <c r="M81" s="14"/>
       <c r="N81" s="14"/>
       <c r="AH81" s="17"/>
       <c r="AI81" s="17"/>
       <c r="AJ81" s="17"/>
     </row>
-    <row r="82" spans="13:36">
+    <row r="82" spans="13:36" x14ac:dyDescent="0.2">
       <c r="M82" s="14"/>
       <c r="N82" s="14"/>
       <c r="AH82" s="17"/>
       <c r="AI82" s="17"/>
       <c r="AJ82" s="17"/>
     </row>
-    <row r="83" spans="13:36">
+    <row r="83" spans="13:36" x14ac:dyDescent="0.2">
       <c r="M83" s="14"/>
       <c r="N83" s="14"/>
       <c r="AH83" s="17"/>
       <c r="AI83" s="17"/>
       <c r="AJ83" s="17"/>
     </row>
-    <row r="84" spans="13:36">
+    <row r="84" spans="13:36" x14ac:dyDescent="0.2">
       <c r="M84" s="14"/>
       <c r="N84" s="14"/>
       <c r="AH84" s="17"/>
       <c r="AI84" s="17"/>
       <c r="AJ84" s="17"/>
     </row>
-    <row r="85" spans="13:36">
+    <row r="85" spans="13:36" x14ac:dyDescent="0.2">
       <c r="M85" s="14"/>
       <c r="N85" s="14"/>
       <c r="AH85" s="17"/>
       <c r="AI85" s="17"/>
       <c r="AJ85" s="17"/>
     </row>
-    <row r="86" spans="13:36">
+    <row r="86" spans="13:36" x14ac:dyDescent="0.2">
       <c r="M86" s="14"/>
       <c r="N86" s="14"/>
       <c r="AH86" s="17"/>
       <c r="AI86" s="17"/>
       <c r="AJ86" s="17"/>
     </row>
-    <row r="87" spans="13:36">
+    <row r="87" spans="13:36" x14ac:dyDescent="0.2">
       <c r="M87" s="14"/>
       <c r="N87" s="14"/>
       <c r="AH87" s="17"/>
       <c r="AI87" s="17"/>
       <c r="AJ87" s="17"/>
     </row>
-    <row r="88" spans="13:36">
+    <row r="88" spans="13:36" x14ac:dyDescent="0.2">
       <c r="M88" s="14"/>
       <c r="N88" s="14"/>
       <c r="AH88" s="17"/>
       <c r="AI88" s="17"/>
       <c r="AJ88" s="17"/>
     </row>
-    <row r="89" spans="13:36">
+    <row r="89" spans="13:36" x14ac:dyDescent="0.2">
       <c r="M89" s="14"/>
       <c r="N89" s="14"/>
       <c r="AH89" s="17"/>
       <c r="AI89" s="17"/>
       <c r="AJ89" s="17"/>
     </row>
-    <row r="90" spans="13:36">
+    <row r="90" spans="13:36" x14ac:dyDescent="0.2">
       <c r="M90" s="14"/>
       <c r="N90" s="14"/>
       <c r="AH90" s="17"/>
       <c r="AI90" s="17"/>
       <c r="AJ90" s="17"/>
     </row>
-    <row r="91" spans="13:36">
+    <row r="91" spans="13:36" x14ac:dyDescent="0.2">
       <c r="M91" s="14"/>
       <c r="N91" s="14"/>
       <c r="AH91" s="17"/>
       <c r="AI91" s="17"/>
       <c r="AJ91" s="17"/>
     </row>
-    <row r="92" spans="13:36">
+    <row r="92" spans="13:36" x14ac:dyDescent="0.2">
       <c r="M92" s="14"/>
       <c r="N92" s="14"/>
       <c r="AH92" s="17"/>
       <c r="AI92" s="17"/>
       <c r="AJ92" s="17"/>
     </row>
-    <row r="93" spans="13:36">
+    <row r="93" spans="13:36" x14ac:dyDescent="0.2">
       <c r="M93" s="14"/>
       <c r="N93" s="14"/>
       <c r="AH93" s="17"/>
       <c r="AI93" s="17"/>
       <c r="AJ93" s="17"/>
     </row>
-    <row r="94" spans="13:36">
+    <row r="94" spans="13:36" x14ac:dyDescent="0.2">
       <c r="M94" s="14"/>
       <c r="N94" s="14"/>
       <c r="AH94" s="17"/>
       <c r="AI94" s="17"/>
       <c r="AJ94" s="17"/>
     </row>
-    <row r="95" spans="13:36">
+    <row r="95" spans="13:36" x14ac:dyDescent="0.2">
       <c r="M95" s="14"/>
       <c r="N95" s="14"/>
       <c r="AH95" s="17"/>
       <c r="AI95" s="17"/>
       <c r="AJ95" s="17"/>
     </row>
-    <row r="96" spans="13:36">
+    <row r="96" spans="13:36" x14ac:dyDescent="0.2">
       <c r="M96" s="14"/>
       <c r="N96" s="14"/>
       <c r="AH96" s="17"/>
       <c r="AI96" s="17"/>
       <c r="AJ96" s="17"/>
     </row>
-    <row r="97" spans="1:36">
+    <row r="97" spans="1:29" x14ac:dyDescent="0.2">
       <c r="M97" s="14"/>
       <c r="N97" s="14"/>
     </row>
-    <row r="98" spans="1:36">
+    <row r="98" spans="1:29" x14ac:dyDescent="0.2">
       <c r="M98" s="14"/>
       <c r="N98" s="14"/>
     </row>
-    <row r="99" spans="1:36">
+    <row r="99" spans="1:29" x14ac:dyDescent="0.2">
       <c r="M99" s="14"/>
       <c r="N99" s="14"/>
     </row>
-    <row r="100" spans="1:36">
+    <row r="100" spans="1:29" x14ac:dyDescent="0.2">
       <c r="M100" s="14"/>
       <c r="N100" s="14"/>
     </row>
-    <row r="101" spans="1:36">
+    <row r="101" spans="1:29" x14ac:dyDescent="0.2">
       <c r="M101" s="14"/>
       <c r="N101" s="14"/>
     </row>
-    <row r="102" spans="1:36" s="17" customFormat="1">
+    <row r="102" spans="1:29" s="17" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A102" s="12"/>
       <c r="B102" s="14"/>
       <c r="C102" s="12"/>
-      <c r="J102" s="17">
-        <f>AVERAGE(J34:J101)</f>
-        <v>0.84323529411764708</v>
-      </c>
-      <c r="O102" s="17">
-        <f>AVERAGE(O34:O101)</f>
-        <v>0.84202981063543803</v>
-      </c>
       <c r="Q102" s="12"/>
-      <c r="S102" s="17">
-        <f>AVERAGE(S34:S101)</f>
-        <v>0.92088235294117637</v>
-      </c>
-      <c r="U102" s="17">
-        <f>AVERAGE(U34:U101)</f>
-        <v>0.83029322306931774</v>
-      </c>
-      <c r="W102" s="17">
-        <f>AVERAGE(W34:W101)</f>
-        <v>0.83997988364710652</v>
-      </c>
-      <c r="AA102" s="17">
-        <f>AVERAGE(AA34:AA101)</f>
-        <v>0.82109379104731384</v>
-      </c>
-      <c r="AC102" s="17">
-        <f>AVERAGE(AC34:AC101)</f>
-        <v>0.80753358799341635</v>
-      </c>
-      <c r="AD102" s="17">
-        <f t="shared" ref="AD102:AE102" si="37">AVERAGE(AD34:AD101)</f>
-        <v>0.12352941176470586</v>
-      </c>
-      <c r="AE102" s="17">
-        <f t="shared" si="37"/>
-        <v>5.8900276809409985E-2</v>
-      </c>
-      <c r="AF102" s="17">
-        <f t="shared" ref="AF102" si="38">AVERAGE(AF34:AF101)</f>
-        <v>4.3688813912789372E-2</v>
-      </c>
-      <c r="AG102" s="17">
-        <f t="shared" ref="AG102" si="39">AVERAGE(AG34:AG101)</f>
-        <v>4.337805986072546E-2</v>
-      </c>
-      <c r="AH102" s="17">
-        <f>AVERAGE(AH2:AH101)</f>
-        <v>234.1</v>
-      </c>
-      <c r="AI102" s="17">
-        <f t="shared" ref="AI102:AJ102" si="40">AVERAGE(AI2:AI101)</f>
-        <v>200.35999999999996</v>
-      </c>
-      <c r="AJ102" s="17">
-        <f t="shared" si="40"/>
-        <v>367.8346769185269</v>
-      </c>
-    </row>
-    <row r="103" spans="1:36">
-      <c r="J103" s="12">
-        <f>COUNTIF(J35:J102,"&gt;1")</f>
-        <v>2</v>
-      </c>
+    </row>
+    <row r="103" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="J103" s="12"/>
       <c r="M103" s="14"/>
       <c r="N103" s="14"/>
-      <c r="O103" s="12">
-        <f>COUNTIF(O35:O102,"&gt;1")</f>
-        <v>2</v>
-      </c>
-      <c r="S103" s="12">
-        <f>COUNTIF(S35:S102,"&gt;1")</f>
-        <v>8</v>
-      </c>
-      <c r="U103" s="17">
-        <f>COUNTIF(U35:U102,"&gt;1")</f>
-        <v>0</v>
-      </c>
-      <c r="W103" s="12">
-        <f>COUNTIF(W35:W102,"&gt;1")</f>
-        <v>0</v>
-      </c>
+      <c r="O103" s="12"/>
+      <c r="S103" s="12"/>
+      <c r="U103" s="17"/>
+      <c r="W103" s="12"/>
       <c r="Y103" s="12"/>
-      <c r="AA103" s="17">
-        <f>COUNTIF(AA35:AA102,"&gt;1")</f>
-        <v>0</v>
-      </c>
-      <c r="AC103" s="17">
-        <f>COUNTIF(AC35:AC102,"&gt;1")</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="104" spans="1:36">
-      <c r="J104" s="18">
-        <f>_xlfn.STDEV.S(J34:J101)</f>
-        <v>8.2745340919294461E-2</v>
-      </c>
+      <c r="AC103" s="17"/>
+    </row>
+    <row r="104" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="J104" s="18"/>
       <c r="K104" s="18"/>
       <c r="L104" s="18"/>
       <c r="M104" s="18"/>
       <c r="N104" s="18"/>
-      <c r="O104" s="18">
-        <f>_xlfn.STDEV.S(O34:O101)</f>
-        <v>8.33392146228117E-2</v>
-      </c>
+      <c r="O104" s="18"/>
       <c r="P104" s="18"/>
       <c r="R104" s="18"/>
-      <c r="S104" s="18">
-        <f>_xlfn.STDEV.S(S34:S101)</f>
-        <v>0.19001383756722384</v>
-      </c>
+      <c r="S104" s="18"/>
       <c r="T104" s="18"/>
-      <c r="U104" s="18">
-        <f>_xlfn.STDEV.S(U34:U101)</f>
-        <v>4.4284040809568284E-2</v>
-      </c>
       <c r="V104" s="18"/>
-      <c r="W104" s="18">
-        <f>_xlfn.STDEV.S(W34:W101)</f>
-        <v>5.3352426173277276E-2</v>
-      </c>
       <c r="X104" s="18"/>
       <c r="Z104" s="18"/>
-      <c r="AA104" s="18">
-        <f>_xlfn.STDEV.S(AA34:AA101)</f>
-        <v>7.8842264501069362E-2</v>
-      </c>
-      <c r="AC104" s="18">
-        <f>_xlfn.STDEV.S(AC34:AC101)</f>
-        <v>7.0743701466331008E-2</v>
-      </c>
-    </row>
-    <row r="105" spans="1:36">
+      <c r="AA104" s="18"/>
+      <c r="AC104" s="18"/>
+    </row>
+    <row r="105" spans="1:29" x14ac:dyDescent="0.2">
       <c r="J105" s="18"/>
       <c r="K105" s="18"/>
       <c r="L105" s="18"/>
@@ -8943,402 +8859,220 @@
       <c r="Z105" s="18"/>
       <c r="AA105" s="18"/>
     </row>
-    <row r="106" spans="1:36" s="17" customFormat="1">
+    <row r="106" spans="1:29" s="17" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A106" s="12"/>
       <c r="B106" s="14"/>
     </row>
-    <row r="107" spans="1:36">
+    <row r="107" spans="1:29" x14ac:dyDescent="0.2">
       <c r="M107" s="14"/>
       <c r="N107" s="14"/>
     </row>
-    <row r="108" spans="1:36">
-      <c r="C108" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="D108" s="17">
-        <f t="shared" ref="D108:D114" si="41">AVERAGE(D33,D40,D47,D54,D61,D68)</f>
-        <v>2101.6</v>
-      </c>
-      <c r="J108" s="17">
-        <f t="shared" ref="J108:J114" si="42">AVERAGE(J33,J40,J47,J54,J61,J68)</f>
-        <v>0.90800000000000003</v>
-      </c>
+    <row r="108" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="D108" s="17"/>
+      <c r="J108" s="17"/>
       <c r="M108" s="14"/>
       <c r="N108" s="14"/>
-      <c r="Q108" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="S108" s="17">
-        <f t="shared" ref="S108:S114" si="43">AVERAGE(S33,S40,S47,S54,S61,S68)</f>
-        <v>0.96500000000000008</v>
-      </c>
-      <c r="U108" s="17">
-        <f t="shared" ref="U108:U114" si="44">AVERAGE(U33,U40,U47,U54,U61,U68)</f>
-        <v>0.84266109093327191</v>
-      </c>
-      <c r="W108" s="17">
-        <f t="shared" ref="W108:W114" si="45">AVERAGE(W33,W40,W47,W54,W61,W68)</f>
-        <v>0.84377906112742129</v>
-      </c>
-      <c r="AA108" s="17">
-        <f t="shared" ref="AA108:AA114" si="46">AVERAGE(AA33,AA40,AA47,AA54,AA61,AA68)</f>
-        <v>0.84058354222541209</v>
-      </c>
-    </row>
-    <row r="109" spans="1:36">
-      <c r="C109" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="D109" s="17">
-        <f t="shared" si="41"/>
-        <v>1946.4</v>
-      </c>
-      <c r="J109" s="17">
-        <f t="shared" si="42"/>
-        <v>0.87999999999999989</v>
-      </c>
+      <c r="U108" s="17"/>
+      <c r="W108" s="17"/>
+    </row>
+    <row r="109" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="D109" s="17"/>
+      <c r="J109" s="17"/>
       <c r="M109" s="14"/>
       <c r="N109" s="14"/>
-      <c r="Q109" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="S109" s="17">
-        <f t="shared" si="43"/>
-        <v>0.96199999999999997</v>
-      </c>
-      <c r="U109" s="17">
-        <f t="shared" si="44"/>
-        <v>0.84188452804600544</v>
-      </c>
-      <c r="W109" s="17">
-        <f t="shared" si="45"/>
-        <v>0.83665427883071142</v>
-      </c>
-      <c r="AA109" s="17">
-        <f t="shared" si="46"/>
-        <v>0.82066351348300337</v>
-      </c>
-    </row>
-    <row r="110" spans="1:36">
-      <c r="C110" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="D110" s="17">
-        <f t="shared" si="41"/>
-        <v>1665.8</v>
-      </c>
-      <c r="J110" s="17">
-        <f t="shared" si="42"/>
-        <v>0.86199999999999988</v>
-      </c>
+      <c r="U109" s="17"/>
+      <c r="W109" s="17"/>
+    </row>
+    <row r="110" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="D110" s="17"/>
+      <c r="J110" s="17"/>
       <c r="M110" s="14"/>
       <c r="N110" s="14"/>
-      <c r="Q110" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="S110" s="17">
-        <f t="shared" si="43"/>
-        <v>0.88000000000000012</v>
-      </c>
-      <c r="U110" s="17">
-        <f t="shared" si="44"/>
-        <v>0.85219847605029808</v>
-      </c>
-      <c r="W110" s="17">
-        <f t="shared" si="45"/>
-        <v>0.83585279066047558</v>
-      </c>
-      <c r="AA110" s="17">
-        <f t="shared" si="46"/>
-        <v>0.8169339025084229</v>
-      </c>
-    </row>
-    <row r="111" spans="1:36">
+      <c r="U110" s="17"/>
+      <c r="W110" s="17"/>
+    </row>
+    <row r="111" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A111" s="17"/>
-      <c r="C111" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="D111" s="17">
-        <f t="shared" si="41"/>
-        <v>1568.2</v>
-      </c>
-      <c r="J111" s="17">
-        <f t="shared" si="42"/>
-        <v>0.80999999999999994</v>
-      </c>
+      <c r="D111" s="17"/>
+      <c r="J111" s="17"/>
       <c r="M111" s="14"/>
       <c r="N111" s="14"/>
-      <c r="Q111" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="S111" s="17">
-        <f t="shared" si="43"/>
-        <v>0.83399999999999996</v>
-      </c>
-      <c r="U111" s="17">
-        <f t="shared" si="44"/>
-        <v>0.85328075626557442</v>
-      </c>
-      <c r="W111" s="17">
-        <f t="shared" si="45"/>
-        <v>0.84390347839040891</v>
-      </c>
-      <c r="AA111" s="17">
-        <f t="shared" si="46"/>
-        <v>0.81595481536269188</v>
-      </c>
-    </row>
-    <row r="112" spans="1:36">
-      <c r="C112" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="D112" s="17">
-        <f t="shared" si="41"/>
-        <v>1793.6</v>
-      </c>
-      <c r="J112" s="17">
-        <f t="shared" si="42"/>
-        <v>0.78400000000000003</v>
-      </c>
+      <c r="U111" s="17"/>
+      <c r="W111" s="17"/>
+    </row>
+    <row r="112" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="D112" s="17"/>
+      <c r="J112" s="17"/>
       <c r="M112" s="14"/>
       <c r="N112" s="14"/>
-      <c r="Q112" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="S112" s="17">
-        <f t="shared" si="43"/>
-        <v>0.8640000000000001</v>
-      </c>
-      <c r="U112" s="17">
-        <f t="shared" si="44"/>
-        <v>0.81269651215889993</v>
-      </c>
-      <c r="W112" s="17">
-        <f t="shared" si="45"/>
-        <v>0.83623437749266838</v>
-      </c>
-      <c r="AA112" s="17">
-        <f t="shared" si="46"/>
-        <v>0.8188699858935875</v>
-      </c>
-    </row>
-    <row r="113" spans="3:27">
-      <c r="C113" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="D113" s="17">
-        <f t="shared" si="41"/>
-        <v>1688.6</v>
-      </c>
-      <c r="J113" s="17">
-        <f t="shared" si="42"/>
-        <v>0.82</v>
-      </c>
+      <c r="U112" s="17"/>
+      <c r="W112" s="17"/>
+    </row>
+    <row r="113" spans="4:23" x14ac:dyDescent="0.2">
+      <c r="D113" s="17"/>
+      <c r="J113" s="17"/>
       <c r="M113" s="14"/>
       <c r="N113" s="14"/>
-      <c r="Q113" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="S113" s="17">
-        <f t="shared" si="43"/>
-        <v>0.9760000000000002</v>
-      </c>
-      <c r="U113" s="17">
-        <f t="shared" si="44"/>
-        <v>0.80661363055226987</v>
-      </c>
-      <c r="W113" s="17">
-        <f t="shared" si="45"/>
-        <v>0.85200838486468311</v>
-      </c>
-      <c r="AA113" s="17">
-        <f t="shared" si="46"/>
-        <v>0.84129119192000723</v>
-      </c>
-    </row>
-    <row r="114" spans="3:27">
-      <c r="C114" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="D114" s="17">
-        <f t="shared" si="41"/>
-        <v>1606.4</v>
-      </c>
-      <c r="J114" s="17">
-        <f t="shared" si="42"/>
-        <v>0.874</v>
-      </c>
+      <c r="U113" s="17"/>
+      <c r="W113" s="17"/>
+    </row>
+    <row r="114" spans="4:23" x14ac:dyDescent="0.2">
+      <c r="D114" s="17"/>
+      <c r="J114" s="17"/>
       <c r="M114" s="14"/>
       <c r="N114" s="14"/>
-      <c r="Q114" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="S114" s="17">
-        <f t="shared" si="43"/>
-        <v>0.97399999999999998</v>
-      </c>
-      <c r="U114" s="17">
-        <f t="shared" si="44"/>
-        <v>0.80865563490413661</v>
-      </c>
-      <c r="W114" s="17">
-        <f t="shared" si="45"/>
-        <v>0.85157922346195181</v>
-      </c>
-      <c r="AA114" s="17">
-        <f t="shared" si="46"/>
-        <v>0.82792901603206881</v>
-      </c>
-    </row>
-    <row r="115" spans="3:27">
+      <c r="U114" s="17"/>
+      <c r="W114" s="17"/>
+    </row>
+    <row r="115" spans="4:23" x14ac:dyDescent="0.2">
       <c r="M115" s="14"/>
       <c r="N115" s="14"/>
     </row>
-    <row r="116" spans="3:27">
+    <row r="116" spans="4:23" x14ac:dyDescent="0.2">
       <c r="M116" s="14"/>
       <c r="N116" s="14"/>
     </row>
-    <row r="117" spans="3:27">
+    <row r="117" spans="4:23" x14ac:dyDescent="0.2">
       <c r="M117" s="14"/>
       <c r="N117" s="14"/>
     </row>
-    <row r="118" spans="3:27">
+    <row r="118" spans="4:23" x14ac:dyDescent="0.2">
       <c r="M118" s="14"/>
       <c r="N118" s="14"/>
     </row>
-    <row r="119" spans="3:27">
+    <row r="119" spans="4:23" x14ac:dyDescent="0.2">
       <c r="M119" s="14"/>
       <c r="N119" s="14"/>
     </row>
-    <row r="120" spans="3:27">
+    <row r="120" spans="4:23" x14ac:dyDescent="0.2">
       <c r="M120" s="14"/>
       <c r="N120" s="14"/>
     </row>
-    <row r="121" spans="3:27">
+    <row r="121" spans="4:23" x14ac:dyDescent="0.2">
       <c r="M121" s="14"/>
       <c r="N121" s="14"/>
     </row>
-    <row r="122" spans="3:27">
+    <row r="122" spans="4:23" x14ac:dyDescent="0.2">
       <c r="M122" s="14"/>
       <c r="N122" s="14"/>
     </row>
-    <row r="123" spans="3:27">
+    <row r="123" spans="4:23" x14ac:dyDescent="0.2">
       <c r="M123" s="14"/>
       <c r="N123" s="14"/>
     </row>
-    <row r="124" spans="3:27">
+    <row r="124" spans="4:23" x14ac:dyDescent="0.2">
       <c r="M124" s="14"/>
       <c r="N124" s="14"/>
     </row>
-    <row r="125" spans="3:27">
+    <row r="125" spans="4:23" x14ac:dyDescent="0.2">
       <c r="M125" s="14"/>
       <c r="N125" s="14"/>
     </row>
-    <row r="126" spans="3:27">
+    <row r="126" spans="4:23" x14ac:dyDescent="0.2">
       <c r="M126" s="14"/>
       <c r="N126" s="14"/>
     </row>
-    <row r="127" spans="3:27">
+    <row r="127" spans="4:23" x14ac:dyDescent="0.2">
       <c r="M127" s="14"/>
       <c r="N127" s="14"/>
     </row>
-    <row r="128" spans="3:27">
+    <row r="128" spans="4:23" x14ac:dyDescent="0.2">
       <c r="M128" s="14"/>
       <c r="N128" s="14"/>
     </row>
-    <row r="129" spans="13:14">
+    <row r="129" spans="13:14" x14ac:dyDescent="0.2">
       <c r="M129" s="14"/>
       <c r="N129" s="14"/>
     </row>
-    <row r="130" spans="13:14">
+    <row r="130" spans="13:14" x14ac:dyDescent="0.2">
       <c r="M130" s="14"/>
       <c r="N130" s="14"/>
     </row>
-    <row r="131" spans="13:14">
+    <row r="131" spans="13:14" x14ac:dyDescent="0.2">
       <c r="M131" s="14"/>
       <c r="N131" s="14"/>
     </row>
-    <row r="132" spans="13:14">
+    <row r="132" spans="13:14" x14ac:dyDescent="0.2">
       <c r="M132" s="14"/>
       <c r="N132" s="14"/>
     </row>
-    <row r="133" spans="13:14">
+    <row r="133" spans="13:14" x14ac:dyDescent="0.2">
       <c r="M133" s="14"/>
       <c r="N133" s="14"/>
     </row>
-    <row r="134" spans="13:14">
+    <row r="134" spans="13:14" x14ac:dyDescent="0.2">
       <c r="M134" s="14"/>
       <c r="N134" s="14"/>
     </row>
-    <row r="135" spans="13:14">
+    <row r="135" spans="13:14" x14ac:dyDescent="0.2">
       <c r="M135" s="14"/>
       <c r="N135" s="14"/>
     </row>
-    <row r="136" spans="13:14">
+    <row r="136" spans="13:14" x14ac:dyDescent="0.2">
       <c r="M136" s="14"/>
       <c r="N136" s="14"/>
     </row>
-    <row r="137" spans="13:14">
+    <row r="137" spans="13:14" x14ac:dyDescent="0.2">
       <c r="M137" s="14"/>
       <c r="N137" s="14"/>
     </row>
-    <row r="138" spans="13:14">
+    <row r="138" spans="13:14" x14ac:dyDescent="0.2">
       <c r="M138" s="14"/>
       <c r="N138" s="14"/>
     </row>
-    <row r="139" spans="13:14">
+    <row r="139" spans="13:14" x14ac:dyDescent="0.2">
       <c r="M139" s="14"/>
       <c r="N139" s="14"/>
     </row>
-    <row r="140" spans="13:14">
+    <row r="140" spans="13:14" x14ac:dyDescent="0.2">
       <c r="M140" s="14"/>
       <c r="N140" s="14"/>
     </row>
-    <row r="141" spans="13:14">
+    <row r="141" spans="13:14" x14ac:dyDescent="0.2">
       <c r="M141" s="14"/>
       <c r="N141" s="14"/>
     </row>
-    <row r="142" spans="13:14">
+    <row r="142" spans="13:14" x14ac:dyDescent="0.2">
       <c r="M142" s="14"/>
       <c r="N142" s="14"/>
     </row>
-    <row r="143" spans="13:14">
+    <row r="143" spans="13:14" x14ac:dyDescent="0.2">
       <c r="M143" s="14"/>
       <c r="N143" s="14"/>
     </row>
-    <row r="144" spans="13:14">
+    <row r="144" spans="13:14" x14ac:dyDescent="0.2">
       <c r="M144" s="14"/>
       <c r="N144" s="14"/>
     </row>
-    <row r="145" spans="13:14">
+    <row r="145" spans="13:14" x14ac:dyDescent="0.2">
       <c r="M145" s="14"/>
       <c r="N145" s="14"/>
     </row>
-    <row r="146" spans="13:14">
+    <row r="146" spans="13:14" x14ac:dyDescent="0.2">
       <c r="M146" s="14"/>
       <c r="N146" s="14"/>
     </row>
-    <row r="147" spans="13:14">
+    <row r="147" spans="13:14" x14ac:dyDescent="0.2">
       <c r="M147" s="14"/>
       <c r="N147" s="14"/>
     </row>
-    <row r="148" spans="13:14">
+    <row r="148" spans="13:14" x14ac:dyDescent="0.2">
       <c r="M148" s="14"/>
       <c r="N148" s="14"/>
     </row>
-    <row r="149" spans="13:14">
+    <row r="149" spans="13:14" x14ac:dyDescent="0.2">
       <c r="M149" s="14"/>
       <c r="N149" s="14"/>
     </row>
-    <row r="150" spans="13:14">
+    <row r="150" spans="13:14" x14ac:dyDescent="0.2">
       <c r="M150" s="14"/>
       <c r="N150" s="14"/>
     </row>
-    <row r="151" spans="13:14">
+    <row r="151" spans="13:14" x14ac:dyDescent="0.2">
       <c r="M151" s="14"/>
       <c r="N151" s="14"/>
     </row>
-    <row r="152" spans="13:14">
+    <row r="152" spans="13:14" x14ac:dyDescent="0.2">
       <c r="M152" s="14"/>
       <c r="N152" s="14"/>
     </row>
@@ -9349,281 +9083,281 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.6"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="11.07421875" style="1"/>
-    <col min="4" max="7" width="11.07421875" style="2"/>
+    <col min="3" max="3" width="11" style="1"/>
+    <col min="4" max="7" width="11" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="31" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="B1" s="31" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="C1" s="32" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="D1" s="32" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="E1" s="33" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="F1" s="33" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="G1" s="33" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="H1" s="33" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8">
-      <c r="A2" t="str">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2">
         <f>Nowcast_R!C112</f>
-        <v>Montag</v>
-      </c>
-      <c r="B2" t="str">
+        <v>0</v>
+      </c>
+      <c r="B2">
         <f>Nowcast_R!Q112</f>
-        <v>Freitag</v>
+        <v>0</v>
       </c>
       <c r="C2" s="1">
         <f>Nowcast_R!D112</f>
-        <v>1793.6</v>
+        <v>0</v>
       </c>
       <c r="D2" s="30">
         <f>Nowcast_R!J112</f>
-        <v>0.78400000000000003</v>
+        <v>0</v>
       </c>
       <c r="E2" s="2">
         <f>Nowcast_R!U112</f>
-        <v>0.81269651215889993</v>
+        <v>0</v>
       </c>
       <c r="F2" s="2">
         <f>Nowcast_R!W112</f>
-        <v>0.83623437749266838</v>
+        <v>0</v>
       </c>
       <c r="G2" s="2">
         <f>Nowcast_R!S112</f>
-        <v>0.8640000000000001</v>
+        <v>0</v>
       </c>
       <c r="H2" s="2">
         <f>Nowcast_R!AA112</f>
-        <v>0.8188699858935875</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8">
-      <c r="A3" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3">
         <f>Nowcast_R!C113</f>
-        <v>Dienstag</v>
-      </c>
-      <c r="B3" t="str">
+        <v>0</v>
+      </c>
+      <c r="B3">
         <f>Nowcast_R!Q113</f>
-        <v>Samstag</v>
+        <v>0</v>
       </c>
       <c r="C3" s="1">
         <f>Nowcast_R!D113</f>
-        <v>1688.6</v>
+        <v>0</v>
       </c>
       <c r="D3" s="2">
         <f>Nowcast_R!J113</f>
-        <v>0.82</v>
+        <v>0</v>
       </c>
       <c r="E3" s="2">
         <f>Nowcast_R!U113</f>
-        <v>0.80661363055226987</v>
+        <v>0</v>
       </c>
       <c r="F3" s="2">
         <f>Nowcast_R!W113</f>
-        <v>0.85200838486468311</v>
+        <v>0</v>
       </c>
       <c r="G3" s="2">
         <f>Nowcast_R!S113</f>
-        <v>0.9760000000000002</v>
+        <v>0</v>
       </c>
       <c r="H3" s="2">
         <f>Nowcast_R!AA113</f>
-        <v>0.84129119192000723</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8">
-      <c r="A4" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4">
         <f>Nowcast_R!C114</f>
-        <v>Mittwoch</v>
-      </c>
-      <c r="B4" t="str">
+        <v>0</v>
+      </c>
+      <c r="B4">
         <f>Nowcast_R!Q114</f>
-        <v>Sonntag</v>
+        <v>0</v>
       </c>
       <c r="C4" s="1">
         <f>Nowcast_R!D114</f>
-        <v>1606.4</v>
+        <v>0</v>
       </c>
       <c r="D4" s="2">
         <f>Nowcast_R!J114</f>
-        <v>0.874</v>
+        <v>0</v>
       </c>
       <c r="E4" s="2">
         <f>Nowcast_R!U114</f>
-        <v>0.80865563490413661</v>
+        <v>0</v>
       </c>
       <c r="F4" s="2">
         <f>Nowcast_R!W114</f>
-        <v>0.85157922346195181</v>
+        <v>0</v>
       </c>
       <c r="G4" s="30">
         <f>Nowcast_R!S114</f>
-        <v>0.97399999999999998</v>
+        <v>0</v>
       </c>
       <c r="H4" s="2">
         <f>Nowcast_R!AA114</f>
-        <v>0.82792901603206881</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8">
-      <c r="A5" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5">
         <f>Nowcast_R!C108</f>
-        <v>Donnerstag</v>
-      </c>
-      <c r="B5" t="str">
+        <v>0</v>
+      </c>
+      <c r="B5">
         <f>Nowcast_R!Q108</f>
-        <v>Montag</v>
+        <v>0</v>
       </c>
       <c r="C5" s="1">
         <f>Nowcast_R!D108</f>
-        <v>2101.6</v>
+        <v>0</v>
       </c>
       <c r="D5" s="30">
         <f>Nowcast_R!J108</f>
-        <v>0.90800000000000003</v>
+        <v>0</v>
       </c>
       <c r="E5" s="2">
         <f>Nowcast_R!U108</f>
-        <v>0.84266109093327191</v>
+        <v>0</v>
       </c>
       <c r="F5" s="2">
         <f>Nowcast_R!W108</f>
-        <v>0.84377906112742129</v>
+        <v>0</v>
       </c>
       <c r="G5" s="30">
         <f>Nowcast_R!S108</f>
-        <v>0.96500000000000008</v>
+        <v>0</v>
       </c>
       <c r="H5" s="2">
         <f>Nowcast_R!AA108</f>
-        <v>0.84058354222541209</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8">
-      <c r="A6" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6">
         <f>Nowcast_R!C109</f>
-        <v>Freitag</v>
-      </c>
-      <c r="B6" t="str">
+        <v>0</v>
+      </c>
+      <c r="B6">
         <f>Nowcast_R!Q109</f>
-        <v>Dienstag</v>
+        <v>0</v>
       </c>
       <c r="C6" s="1">
         <f>Nowcast_R!D109</f>
-        <v>1946.4</v>
+        <v>0</v>
       </c>
       <c r="D6" s="2">
         <f>Nowcast_R!J109</f>
-        <v>0.87999999999999989</v>
+        <v>0</v>
       </c>
       <c r="E6" s="2">
         <f>Nowcast_R!U109</f>
-        <v>0.84188452804600544</v>
+        <v>0</v>
       </c>
       <c r="F6" s="2">
         <f>Nowcast_R!W109</f>
-        <v>0.83665427883071142</v>
+        <v>0</v>
       </c>
       <c r="G6" s="2">
         <f>Nowcast_R!S109</f>
-        <v>0.96199999999999997</v>
+        <v>0</v>
       </c>
       <c r="H6" s="2">
         <f>Nowcast_R!AA109</f>
-        <v>0.82066351348300337</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8">
-      <c r="A7" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7">
         <f>Nowcast_R!C110</f>
-        <v>Samstag</v>
-      </c>
-      <c r="B7" t="str">
+        <v>0</v>
+      </c>
+      <c r="B7">
         <f>Nowcast_R!Q110</f>
-        <v>Mittwoch</v>
+        <v>0</v>
       </c>
       <c r="C7" s="1">
         <f>Nowcast_R!D110</f>
-        <v>1665.8</v>
+        <v>0</v>
       </c>
       <c r="D7" s="2">
         <f>Nowcast_R!J110</f>
-        <v>0.86199999999999988</v>
+        <v>0</v>
       </c>
       <c r="E7" s="2">
         <f>Nowcast_R!U110</f>
-        <v>0.85219847605029808</v>
+        <v>0</v>
       </c>
       <c r="F7" s="2">
         <f>Nowcast_R!W110</f>
-        <v>0.83585279066047558</v>
+        <v>0</v>
       </c>
       <c r="G7" s="2">
         <f>Nowcast_R!S110</f>
-        <v>0.88000000000000012</v>
+        <v>0</v>
       </c>
       <c r="H7" s="2">
         <f>Nowcast_R!AA110</f>
-        <v>0.8169339025084229</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8">
-      <c r="A8" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8">
         <f>Nowcast_R!C111</f>
-        <v>Sonntag</v>
-      </c>
-      <c r="B8" t="str">
+        <v>0</v>
+      </c>
+      <c r="B8">
         <f>Nowcast_R!Q111</f>
-        <v>Donnerstag</v>
+        <v>0</v>
       </c>
       <c r="C8" s="1">
         <f>Nowcast_R!D111</f>
-        <v>1568.2</v>
+        <v>0</v>
       </c>
       <c r="D8" s="2">
         <f>Nowcast_R!J111</f>
-        <v>0.80999999999999994</v>
+        <v>0</v>
       </c>
       <c r="E8" s="2">
         <f>Nowcast_R!U111</f>
-        <v>0.85328075626557442</v>
+        <v>0</v>
       </c>
       <c r="F8" s="2">
         <f>Nowcast_R!W111</f>
-        <v>0.84390347839040891</v>
+        <v>0</v>
       </c>
       <c r="G8" s="30">
         <f>Nowcast_R!S111</f>
-        <v>0.83399999999999996</v>
+        <v>0</v>
       </c>
       <c r="H8" s="2">
         <f>Nowcast_R!AA111</f>
-        <v>0.81595481536269188</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -9633,19 +9367,19 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.6"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="17.765625" customWidth="1"/>
+    <col min="1" max="1" width="17.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="B1" s="20" t="s">
         <v>6</v>
       </c>
@@ -9662,67 +9396,67 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="B2" s="2">
         <f>Nowcast_R!J102</f>
-        <v>0.84323529411764708</v>
+        <v>0</v>
       </c>
       <c r="C2" s="2">
         <f>Nowcast_R!S102</f>
-        <v>0.92088235294117637</v>
+        <v>0</v>
       </c>
       <c r="D2" s="2">
         <f>Nowcast_R!U102</f>
-        <v>0.83029322306931774</v>
+        <v>0</v>
       </c>
       <c r="E2" s="2">
         <f>Nowcast_R!W102</f>
-        <v>0.83997988364710652</v>
+        <v>0</v>
       </c>
       <c r="F2" s="2">
         <f>Nowcast_R!AA102</f>
-        <v>0.82109379104731384</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="B3" s="2">
         <f>Nowcast_R!J104</f>
-        <v>8.2745340919294461E-2</v>
+        <v>0</v>
       </c>
       <c r="C3" s="2">
         <f>Nowcast_R!S104</f>
-        <v>0.19001383756722384</v>
+        <v>0</v>
       </c>
       <c r="D3" s="2">
         <f>Nowcast_R!U104</f>
-        <v>4.4284040809568284E-2</v>
+        <v>0</v>
       </c>
       <c r="E3" s="2">
         <f>Nowcast_R!W104</f>
-        <v>5.3352426173277276E-2</v>
+        <v>0</v>
       </c>
       <c r="F3" s="2">
         <f>Nowcast_R!AA104</f>
-        <v>7.8842264501069362E-2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" s="1" customFormat="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="32" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="B4" s="1">
         <f>Nowcast_R!J103</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C4" s="1">
         <f>Nowcast_R!S103</f>
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="D4" s="1">
         <f>Nowcast_R!U103</f>
@@ -9743,596 +9477,596 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:D54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+    <sheetView topLeftCell="A40" workbookViewId="0">
       <selection activeCell="B52" sqref="B52"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.6"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="77.69140625" customWidth="1"/>
-    <col min="3" max="3" width="13.69140625" style="48" customWidth="1"/>
-    <col min="4" max="4" width="12.53515625" style="61" customWidth="1"/>
+    <col min="2" max="2" width="77.6640625" customWidth="1"/>
+    <col min="3" max="3" width="13.6640625" style="48" customWidth="1"/>
+    <col min="4" max="4" width="12.5" style="61" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="35" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="35" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="35" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="35" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="35"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="35" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
-      <c r="A3" s="35" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" s="35" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5" s="35" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6" s="35"/>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="A7" s="35" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="44">
         <v>43964</v>
       </c>
       <c r="B8" s="31" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="C8" s="49"/>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="44">
         <v>43966</v>
       </c>
       <c r="B9" s="31" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="C9" s="49"/>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="35"/>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="35" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="31" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="31" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B14" s="31"/>
       <c r="C14" s="49"/>
     </row>
-    <row r="15" spans="1:4" s="58" customFormat="1" ht="46.3" customHeight="1">
+    <row r="15" spans="1:4" s="58" customFormat="1" ht="46.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="56" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="B15" s="56" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="C15" s="57" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="D15" s="62" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="31" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="B16" s="19" t="s">
         <v>9</v>
       </c>
       <c r="C16" s="50" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="D16" s="63" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="31" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="B17" s="36" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="C17" s="51" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="D17" s="63" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="31" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="B18" s="19" t="s">
         <v>5</v>
       </c>
       <c r="C18" s="50" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="D18" s="63" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" s="31" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="B19" s="20" t="s">
         <v>10</v>
       </c>
       <c r="C19" s="50" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="D19" s="63" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A20" s="31" t="s">
+        <v>59</v>
+      </c>
+      <c r="B20" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="C20" s="50" t="s">
+        <v>100</v>
+      </c>
+      <c r="D20" s="63" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A21" s="31" t="s">
         <v>66</v>
       </c>
-      <c r="B20" s="20" t="s">
-        <v>39</v>
-      </c>
-      <c r="C20" s="50" t="s">
-        <v>107</v>
-      </c>
-      <c r="D20" s="63" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4">
-      <c r="A21" s="31" t="s">
-        <v>73</v>
-      </c>
       <c r="B21" s="20" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="C21" s="50" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="D21" s="63" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" s="31" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="B22" s="20" t="s">
         <v>11</v>
       </c>
       <c r="C22" s="50" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="D22" s="63" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A23" s="31" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="B23" s="20" t="s">
         <v>0</v>
       </c>
       <c r="C23" s="50" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="D23" s="63" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A24" s="31" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="B24" s="20" t="s">
         <v>1</v>
       </c>
       <c r="C24" s="50" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="D24" s="63" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A25" s="31" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="B25" s="20" t="s">
         <v>6</v>
       </c>
       <c r="C25" s="50" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="D25" s="63" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A26" s="31" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="B26" s="20" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="C26" s="50" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="D26" s="63" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A27" s="31" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="B27" s="20" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="C27" s="50" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="D27" s="63" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A28" s="31" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="B28" s="21" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="C28" s="51" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="D28" s="63" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A29" s="31" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="B29" s="21" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="C29" s="51" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="D29" s="63" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A30" s="31" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="B30" s="29" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="C30" s="52" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="D30" s="63" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A31" s="31" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="B31" s="22" t="s">
         <v>4</v>
       </c>
       <c r="C31" s="53" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="D31" s="63" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="32" spans="1:4">
+    <row r="32" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A32" s="31" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="B32" s="19" t="s">
         <v>5</v>
       </c>
       <c r="C32" s="50" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="D32" s="63" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A33" s="31" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="B33" s="21" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="C33" s="51" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="D33" s="63" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A34" s="31" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="B34" s="20" t="s">
         <v>7</v>
       </c>
       <c r="C34" s="50" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="D34" s="63" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A35" s="31" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="B35" s="20" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="C35" s="50" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="D35" s="63" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A36" s="31" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="B36" s="29" t="s">
         <v>8</v>
       </c>
       <c r="C36" s="52" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="D36" s="63" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A37" s="31" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="B37" s="20" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="C37" s="50" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="D37" s="63" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A38" s="31" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="B38" s="20" t="s">
         <v>12</v>
       </c>
       <c r="C38" s="50" t="s">
+        <v>100</v>
+      </c>
+      <c r="D38" s="63" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A39" s="31" t="s">
+        <v>81</v>
+      </c>
+      <c r="B39" s="20" t="s">
+        <v>113</v>
+      </c>
+      <c r="C39" s="50" t="s">
+        <v>100</v>
+      </c>
+      <c r="D39" s="63" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A40" s="31" t="s">
+        <v>82</v>
+      </c>
+      <c r="B40" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="C40" s="50" t="s">
+        <v>100</v>
+      </c>
+      <c r="D40" s="63" t="s">
         <v>107</v>
       </c>
-      <c r="D38" s="63" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4">
-      <c r="A39" s="31" t="s">
-        <v>88</v>
-      </c>
-      <c r="B39" s="20" t="s">
-        <v>120</v>
-      </c>
-      <c r="C39" s="50" t="s">
-        <v>107</v>
-      </c>
-      <c r="D39" s="63" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4">
-      <c r="A40" s="31" t="s">
-        <v>89</v>
-      </c>
-      <c r="B40" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="C40" s="50" t="s">
-        <v>107</v>
-      </c>
-      <c r="D40" s="63" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4">
+    </row>
+    <row r="41" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A41" s="31" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="B41" s="20" t="s">
         <v>13</v>
       </c>
       <c r="C41" s="50" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="D41" s="63" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A42" s="31" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="B42" s="29" t="s">
         <v>14</v>
       </c>
       <c r="C42" s="52" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="D42" s="63" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A43" s="31" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="B43" s="20" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="C43" s="50" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="D43" s="63" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A44" s="31" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="B44" s="20" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="C44" s="50" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="D44" s="63" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" s="31"/>
       <c r="B45" s="20"/>
       <c r="C45" s="50"/>
     </row>
-    <row r="46" spans="1:4" s="35" customFormat="1">
+    <row r="46" spans="1:4" s="35" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A46" s="35" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="B46" s="59"/>
       <c r="C46" s="60"/>
       <c r="D46" s="62"/>
     </row>
-    <row r="47" spans="1:4" s="58" customFormat="1" ht="46.3" customHeight="1">
+    <row r="47" spans="1:4" s="58" customFormat="1" ht="46.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="56" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="B47" s="56" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="C47" s="57"/>
       <c r="D47" s="62"/>
     </row>
-    <row r="48" spans="1:4">
+    <row r="48" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A48" s="31" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="B48" s="29" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="C48" s="31"/>
     </row>
-    <row r="49" spans="1:3">
+    <row r="49" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A49" s="31" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="B49" s="34" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="C49" s="55"/>
     </row>
-    <row r="50" spans="1:3">
+    <row r="50" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A50" s="31" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="B50" s="29" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="C50" s="52"/>
     </row>
-    <row r="51" spans="1:3">
+    <row r="51" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A51" s="31" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="B51" s="20" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="C51" s="50"/>
     </row>
-    <row r="52" spans="1:3">
+    <row r="52" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A52" s="31" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="B52" s="19" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="C52" s="54"/>
     </row>
-    <row r="53" spans="1:3">
+    <row r="53" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A53" s="31" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="B53" s="19" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="C53" s="54"/>
     </row>
-    <row r="54" spans="1:3">
+    <row r="54" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A54" s="31" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="B54" s="19" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="C54" s="54"/>
     </row>

</xml_diff>

<commit_message>
refactored & add confirmed cases & evaluation thereof
</commit_message>
<xml_diff>
--- a/data/20200511_Nowcasting_Zahlen.xlsx
+++ b/data/20200511_Nowcasting_Zahlen.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/la5373/Documents/Code/Julia/ReproductionNumbers/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA34B102-3A5F-8440-946F-CD29A8E5FCD8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4AF1749-904B-694F-9943-866425E247AB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15100" windowHeight="25600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15260" windowHeight="25600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Nowcast_R" sheetId="1" r:id="rId1"/>
@@ -933,11 +933,11 @@
   <dimension ref="A1:AJ152"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="N21" activePane="bottomRight" state="frozenSplit"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="U3" activePane="bottomRight" state="frozenSplit"/>
       <selection activeCell="J11" sqref="H9:J11"/>
       <selection pane="topRight" activeCell="K1" sqref="K1"/>
       <selection pane="bottomLeft" activeCell="A12" sqref="A12"/>
-      <selection pane="bottomRight" activeCell="AL95" sqref="A95:AL116"/>
+      <selection pane="bottomRight" activeCell="Z13" sqref="Z13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1287,7 +1287,7 @@
       </c>
       <c r="R5" s="41"/>
       <c r="T5" s="14">
-        <f t="shared" ref="T5:T36" si="3">AVERAGE(D2:D8)</f>
+        <f>AVERAGE(D2:D8)</f>
         <v>668.14285714285711</v>
       </c>
       <c r="U5" s="42"/>
@@ -1355,7 +1355,7 @@
         <v>157</v>
       </c>
       <c r="T6" s="14">
-        <f t="shared" si="3"/>
+        <f t="shared" ref="T5:T36" si="3">AVERAGE(D3:D9)</f>
         <v>908</v>
       </c>
       <c r="U6" s="42"/>
@@ -1566,7 +1566,7 @@
       </c>
       <c r="S9" s="8"/>
       <c r="T9" s="5">
-        <f t="shared" si="3"/>
+        <f>AVERAGE(D6:D12)</f>
         <v>2065.5714285714284</v>
       </c>
       <c r="U9" s="9">
@@ -1576,7 +1576,7 @@
       <c r="V9" s="41"/>
       <c r="W9" s="42"/>
       <c r="X9" s="5">
-        <f t="shared" ref="X9:X63" si="5">AVERAGE(R6:R12)</f>
+        <f>AVERAGE(R6:R12)</f>
         <v>696.14285714285711</v>
       </c>
       <c r="Y9" s="42"/>
@@ -1633,7 +1633,7 @@
         <v>271</v>
       </c>
       <c r="N10" s="5">
-        <f t="shared" ref="N10:N67" si="6">AVERAGE(D7:D10)</f>
+        <f t="shared" ref="N10:N67" si="5">AVERAGE(D7:D10)</f>
         <v>1717</v>
       </c>
       <c r="O10" s="8">
@@ -1656,13 +1656,13 @@
         <v>2580.5714285714284</v>
       </c>
       <c r="U10" s="9">
-        <f t="shared" ref="U10:U64" si="7">T10/T6</f>
+        <f t="shared" ref="U10:U64" si="6">T10/T6</f>
         <v>2.842039018250472</v>
       </c>
       <c r="V10" s="41"/>
       <c r="W10" s="42"/>
       <c r="X10" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" ref="X9:X63" si="7">AVERAGE(R7:R13)</f>
         <v>837.14285714285711</v>
       </c>
       <c r="Y10" s="42"/>
@@ -1719,7 +1719,7 @@
         <v>802</v>
       </c>
       <c r="N11" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>2276.75</v>
       </c>
       <c r="O11" s="8">
@@ -1742,20 +1742,20 @@
         <v>3074.2857142857142</v>
       </c>
       <c r="U11" s="9">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>2.5078662160587344</v>
       </c>
       <c r="V11" s="41"/>
       <c r="W11" s="42"/>
       <c r="X11" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>947.28571428571433</v>
       </c>
       <c r="Y11" s="42"/>
       <c r="Z11" s="41"/>
       <c r="AA11" s="42"/>
       <c r="AB11" s="5">
-        <f t="shared" si="8"/>
+        <f>X18</f>
         <v>3336.5714285714284</v>
       </c>
       <c r="AC11" s="39"/>
@@ -1805,7 +1805,7 @@
         <v>693</v>
       </c>
       <c r="N12" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>2841.75</v>
       </c>
       <c r="O12" s="8">
@@ -1828,7 +1828,7 @@
         <v>3553.8571428571427</v>
       </c>
       <c r="U12" s="9">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>2.1898767605633802</v>
       </c>
       <c r="V12" s="5">
@@ -1840,7 +1840,7 @@
         <v>2.9624409396843423</v>
       </c>
       <c r="X12" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>1232.8571428571429</v>
       </c>
       <c r="Y12" s="42"/>
@@ -1897,7 +1897,7 @@
         <v>733</v>
       </c>
       <c r="N13" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>3437</v>
       </c>
       <c r="O13" s="8">
@@ -1920,7 +1920,7 @@
         <v>4125.8571428571431</v>
       </c>
       <c r="U13" s="9">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>1.9974410401825855</v>
       </c>
       <c r="V13" s="5">
@@ -1932,7 +1932,7 @@
         <v>2.8077573674485339</v>
       </c>
       <c r="X13" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>1556.4285714285713</v>
       </c>
       <c r="Y13" s="9">
@@ -1995,7 +1995,7 @@
         <v>1043</v>
       </c>
       <c r="N14" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>3911</v>
       </c>
       <c r="O14" s="8">
@@ -2018,7 +2018,7 @@
         <v>4513</v>
       </c>
       <c r="U14" s="9">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>1.7488374667847653</v>
       </c>
       <c r="V14" s="5">
@@ -2030,7 +2030,7 @@
         <v>2.4917696780320471</v>
       </c>
       <c r="X14" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>1838.1428571428571</v>
       </c>
       <c r="Y14" s="9">
@@ -2093,7 +2093,7 @@
         <v>1174</v>
       </c>
       <c r="N15" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>4276.75</v>
       </c>
       <c r="O15" s="8">
@@ -2116,7 +2116,7 @@
         <v>4812.5714285714284</v>
       </c>
       <c r="U15" s="9">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>1.5654275092936802</v>
       </c>
       <c r="V15" s="5">
@@ -2128,7 +2128,7 @@
         <v>2.218289784927256</v>
       </c>
       <c r="X15" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>1967.4285714285713</v>
       </c>
       <c r="Y15" s="9">
@@ -2203,7 +2203,7 @@
         <v>1144</v>
       </c>
       <c r="N16" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>4875.25</v>
       </c>
       <c r="O16" s="8">
@@ -2225,7 +2225,7 @@
         <v>4977.1428571428569</v>
       </c>
       <c r="U16" s="9">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>1.4004904128311291</v>
       </c>
       <c r="V16" s="14">
@@ -2237,7 +2237,7 @@
         <v>2.0493155583186722</v>
       </c>
       <c r="X16" s="14">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>2380</v>
       </c>
       <c r="Y16" s="9">
@@ -2245,11 +2245,11 @@
         <v>1.9304750869061413</v>
       </c>
       <c r="Z16" s="14">
-        <f t="shared" ref="Z16:Z66" si="15">AVERAGE(R13:R16,Y13^1.75*R10,Y13^1.75*R11,Y13^1.75*R12)</f>
+        <f>AVERAGE(R13:R16,Y13^1.75*R10,Y13^1.75*R11,Y13^1.75*R12)</f>
         <v>2857.7724440950578</v>
       </c>
       <c r="AA16" s="18">
-        <f t="shared" ref="AA16:AA66" si="16">Z16/X12</f>
+        <f>Z16/X12</f>
         <v>2.3180077762068834</v>
       </c>
       <c r="AB16" s="14">
@@ -2265,11 +2265,11 @@
         <v>1116</v>
       </c>
       <c r="AI16" s="17">
-        <f t="shared" ref="AI16:AI50" si="17">ABS(T16-$D16)</f>
+        <f t="shared" ref="AI16:AI50" si="15">ABS(T16-$D16)</f>
         <v>1013.8571428571431</v>
       </c>
       <c r="AJ16" s="17">
-        <f t="shared" ref="AJ16:AJ50" si="18">ABS(V16-$D16)</f>
+        <f t="shared" ref="AJ16:AJ50" si="16">ABS(V16-$D16)</f>
         <v>1291.9747348990868</v>
       </c>
     </row>
@@ -2316,7 +2316,7 @@
         <v>1042</v>
       </c>
       <c r="N17" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>5098.75</v>
       </c>
       <c r="O17" s="8">
@@ -2338,7 +2338,7 @@
         <v>5112.4285714285716</v>
       </c>
       <c r="U17" s="9">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>1.2391191440739586</v>
       </c>
       <c r="V17" s="14">
@@ -2350,7 +2350,7 @@
         <v>1.7371819977301817</v>
       </c>
       <c r="X17" s="14">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>2897.1428571428573</v>
       </c>
       <c r="Y17" s="9">
@@ -2358,11 +2358,11 @@
         <v>1.8614043139054615</v>
       </c>
       <c r="Z17" s="14">
-        <f t="shared" si="15"/>
+        <f t="shared" ref="Z16:Z66" si="17">AVERAGE(R14:R17,Y14^1.75*R11,Y14^1.75*R12,Y14^1.75*R13)</f>
         <v>3259.668974561363</v>
       </c>
       <c r="AA17" s="18">
-        <f t="shared" si="16"/>
+        <f t="shared" ref="AA16:AA66" si="18">Z17/X13</f>
         <v>2.0943260965515873</v>
       </c>
       <c r="AB17" s="14">
@@ -2378,11 +2378,11 @@
         <v>163</v>
       </c>
       <c r="AI17" s="17">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>149.57142857142844</v>
       </c>
       <c r="AJ17" s="17">
-        <f t="shared" si="18"/>
+        <f t="shared" si="16"/>
         <v>1905.3647537779116</v>
       </c>
     </row>
@@ -2429,7 +2429,7 @@
         <v>2801</v>
       </c>
       <c r="N18" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>5318.75</v>
       </c>
       <c r="O18" s="8">
@@ -2451,7 +2451,7 @@
         <v>5118.5714285714284</v>
       </c>
       <c r="U18" s="9">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>1.1341837865214777</v>
       </c>
       <c r="V18" s="14">
@@ -2463,7 +2463,7 @@
         <v>1.534288574975726</v>
       </c>
       <c r="X18" s="14">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>3336.5714285714284</v>
       </c>
       <c r="Y18" s="9">
@@ -2471,11 +2471,11 @@
         <v>1.8151861350742209</v>
       </c>
       <c r="Z18" s="14">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>3212.1649078104065</v>
       </c>
       <c r="AA18" s="18">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>1.7475055844153917</v>
       </c>
       <c r="AB18" s="14">
@@ -2491,11 +2491,11 @@
         <v>9</v>
       </c>
       <c r="AI18" s="17">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>209.42857142857156</v>
       </c>
       <c r="AJ18" s="17">
-        <f t="shared" si="18"/>
+        <f t="shared" si="16"/>
         <v>1596.244338865451</v>
       </c>
     </row>
@@ -2542,7 +2542,7 @@
         <v>2958</v>
       </c>
       <c r="N19" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>5332.5</v>
       </c>
       <c r="O19" s="8">
@@ -2564,7 +2564,7 @@
         <v>5004.7142857142853</v>
       </c>
       <c r="U19" s="9">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>1.0399251959154594</v>
       </c>
       <c r="V19" s="14">
@@ -2576,7 +2576,7 @@
         <v>1.3562165329570601</v>
       </c>
       <c r="X19" s="14">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>3644.1428571428573</v>
       </c>
       <c r="Y19" s="9">
@@ -2584,11 +2584,11 @@
         <v>1.8522364217252398</v>
       </c>
       <c r="Z19" s="14">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>3920.0137594175749</v>
       </c>
       <c r="AA19" s="18">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>1.9924554397272021</v>
       </c>
       <c r="AB19" s="14">
@@ -2604,11 +2604,11 @@
         <v>584</v>
       </c>
       <c r="AI19" s="17">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>255.71428571428532</v>
       </c>
       <c r="AJ19" s="17">
-        <f t="shared" si="18"/>
+        <f t="shared" si="16"/>
         <v>1777.888937465349</v>
       </c>
     </row>
@@ -2655,7 +2655,7 @@
         <v>2705</v>
       </c>
       <c r="N20" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>5163.5</v>
       </c>
       <c r="O20" s="8">
@@ -2677,7 +2677,7 @@
         <v>4889.2857142857147</v>
       </c>
       <c r="U20" s="9">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>0.9823478760045925</v>
       </c>
       <c r="V20" s="14">
@@ -2689,7 +2689,7 @@
         <v>1.2249373842147615</v>
       </c>
       <c r="X20" s="14">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>4047.2857142857142</v>
       </c>
       <c r="Y20" s="9">
@@ -2697,11 +2697,11 @@
         <v>1.7005402160864345</v>
       </c>
       <c r="Z20" s="14">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>4807.5847769659285</v>
       </c>
       <c r="AA20" s="18">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>2.0199936037671971</v>
       </c>
       <c r="AB20" s="14">
@@ -2717,11 +2717,11 @@
         <v>151</v>
       </c>
       <c r="AI20" s="17">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>425.71428571428532</v>
       </c>
       <c r="AJ20" s="17">
-        <f t="shared" si="18"/>
+        <f t="shared" si="16"/>
         <v>781.68835229175511</v>
       </c>
     </row>
@@ -2768,7 +2768,7 @@
         <v>1948</v>
       </c>
       <c r="N21" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>4970.75</v>
       </c>
       <c r="O21" s="8">
@@ -2790,7 +2790,7 @@
         <v>4732.5714285714284</v>
       </c>
       <c r="U21" s="9">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>0.92569927627350712</v>
       </c>
       <c r="V21" s="14">
@@ -2802,7 +2802,7 @@
         <v>1.111048875931103</v>
       </c>
       <c r="X21" s="14">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>4560</v>
       </c>
       <c r="Y21" s="9">
@@ -2810,11 +2810,11 @@
         <v>1.5739644970414199</v>
       </c>
       <c r="Z21" s="14">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>5559.7634576747687</v>
       </c>
       <c r="AA21" s="18">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>1.9190505031421785</v>
       </c>
       <c r="AB21" s="14">
@@ -2830,11 +2830,11 @@
         <v>480</v>
       </c>
       <c r="AI21" s="17">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>241.57142857142844</v>
       </c>
       <c r="AJ21" s="17">
-        <f t="shared" si="18"/>
+        <f t="shared" si="16"/>
         <v>1189.1580175637691</v>
       </c>
     </row>
@@ -2881,7 +2881,7 @@
         <v>4062</v>
       </c>
       <c r="N22" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>4613</v>
       </c>
       <c r="O22" s="8">
@@ -2903,7 +2903,7 @@
         <v>4601</v>
       </c>
       <c r="U22" s="9">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>0.89888361708065867</v>
       </c>
       <c r="V22" s="14">
@@ -2915,7 +2915,7 @@
         <v>1.0105717951757507</v>
       </c>
       <c r="X22" s="14">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>4848.1428571428569</v>
       </c>
       <c r="Y22" s="9">
@@ -2923,11 +2923,11 @@
         <v>1.4530313409830451</v>
       </c>
       <c r="Z22" s="14">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>5754.370861923986</v>
       </c>
       <c r="AA22" s="18">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>1.7246358979905765</v>
       </c>
       <c r="AB22" s="14">
@@ -2943,11 +2943,11 @@
         <v>716</v>
       </c>
       <c r="AI22" s="17">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>704</v>
       </c>
       <c r="AJ22" s="17">
-        <f t="shared" si="18"/>
+        <f t="shared" si="16"/>
         <v>1275.6839173067347</v>
       </c>
     </row>
@@ -2994,7 +2994,7 @@
         <v>4764</v>
       </c>
       <c r="N23" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>4721.5</v>
       </c>
       <c r="O23" s="8">
@@ -3017,7 +3017,7 @@
         <v>4500</v>
       </c>
       <c r="U23" s="9">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>0.89915222789940918</v>
       </c>
       <c r="V23" s="5">
@@ -3029,7 +3029,7 @@
         <v>0.96350015330148953</v>
       </c>
       <c r="X23" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>4946.5714285714284</v>
       </c>
       <c r="Y23" s="9">
@@ -3037,11 +3037,11 @@
         <v>1.3574032694343172</v>
       </c>
       <c r="Z23" s="5">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>5955.0858367168721</v>
       </c>
       <c r="AA23" s="9">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>1.63415268560187</v>
       </c>
       <c r="AB23" s="5">
@@ -3059,11 +3059,11 @@
         <v>461</v>
       </c>
       <c r="AI23" s="17">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>683</v>
       </c>
       <c r="AJ23" s="17">
-        <f t="shared" si="18"/>
+        <f t="shared" si="16"/>
         <v>360.95701848413137</v>
       </c>
     </row>
@@ -3110,7 +3110,7 @@
         <v>4118</v>
       </c>
       <c r="N24" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>4434</v>
       </c>
       <c r="O24" s="8">
@@ -3133,7 +3133,7 @@
         <v>4331.7142857142853</v>
       </c>
       <c r="U24" s="9">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>0.88596055514974414</v>
       </c>
       <c r="V24" s="5">
@@ -3145,7 +3145,7 @@
         <v>0.91111038219010831</v>
       </c>
       <c r="X24" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>4925.2857142857147</v>
       </c>
       <c r="Y24" s="9">
@@ -3153,11 +3153,11 @@
         <v>1.2169355123363101</v>
       </c>
       <c r="Z24" s="5">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>6425.0962950039748</v>
       </c>
       <c r="AA24" s="9">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>1.5875074676159622</v>
       </c>
       <c r="AB24" s="5">
@@ -3175,11 +3175,11 @@
         <v>269</v>
       </c>
       <c r="AI24" s="17">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>166.71428571428532</v>
       </c>
       <c r="AJ24" s="17">
-        <f t="shared" si="18"/>
+        <f t="shared" si="16"/>
         <v>289.67897577949407</v>
       </c>
     </row>
@@ -3226,7 +3226,7 @@
         <v>4954</v>
       </c>
       <c r="N25" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>4413</v>
       </c>
       <c r="O25" s="8">
@@ -3249,7 +3249,7 @@
         <v>4248.8571428571431</v>
       </c>
       <c r="U25" s="9">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>0.89779038879497719</v>
       </c>
       <c r="V25" s="5">
@@ -3261,7 +3261,7 @@
         <v>0.89742668704440265</v>
       </c>
       <c r="X25" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>5116</v>
       </c>
       <c r="Y25" s="9">
@@ -3269,11 +3269,11 @@
         <v>1.1219298245614036</v>
       </c>
       <c r="Z25" s="5">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>6554.9175496124471</v>
       </c>
       <c r="AA25" s="9">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>1.4374819187746595</v>
       </c>
       <c r="AB25" s="5">
@@ -3291,11 +3291,11 @@
         <v>6</v>
       </c>
       <c r="AI25" s="17">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>158.14285714285688</v>
       </c>
       <c r="AJ25" s="17">
-        <f t="shared" si="18"/>
+        <f t="shared" si="16"/>
         <v>159.86410165614689</v>
       </c>
     </row>
@@ -3342,7 +3342,7 @@
         <v>5780</v>
       </c>
       <c r="N26" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>4449.25</v>
       </c>
       <c r="O26" s="8">
@@ -3365,7 +3365,7 @@
         <v>4170.8571428571431</v>
       </c>
       <c r="U26" s="9">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>0.90651100692396069</v>
       </c>
       <c r="V26" s="5">
@@ -3377,7 +3377,7 @@
         <v>0.90582470697368356</v>
       </c>
       <c r="X26" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>5287.7142857142853</v>
       </c>
       <c r="Y26" s="9">
@@ -3385,11 +3385,11 @@
         <v>1.0906680024751745</v>
       </c>
       <c r="Z26" s="5">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>6344.0621064468269</v>
       </c>
       <c r="AA26" s="9">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>1.3085551093239765</v>
       </c>
       <c r="AB26" s="5">
@@ -3407,11 +3407,11 @@
         <v>407</v>
       </c>
       <c r="AI26" s="17">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>128.85714285714312</v>
       </c>
       <c r="AJ26" s="17">
-        <f t="shared" si="18"/>
+        <f t="shared" si="16"/>
         <v>125.6994767859178</v>
       </c>
     </row>
@@ -3458,7 +3458,7 @@
         <v>6294</v>
       </c>
       <c r="N27" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>4187.75</v>
       </c>
       <c r="O27" s="8">
@@ -3481,7 +3481,7 @@
         <v>4052</v>
       </c>
       <c r="U27" s="9">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>0.90044444444444449</v>
       </c>
       <c r="V27" s="5">
@@ -3493,7 +3493,7 @@
         <v>0.88033691606502285</v>
       </c>
       <c r="X27" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>5344</v>
       </c>
       <c r="Y27" s="9">
@@ -3501,11 +3501,11 @@
         <v>1.08034424998556</v>
       </c>
       <c r="Z27" s="5">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>5795.1825488292307</v>
       </c>
       <c r="AA27" s="9">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>1.1715554162133834</v>
       </c>
       <c r="AB27" s="5">
@@ -3523,11 +3523,11 @@
         <v>51</v>
       </c>
       <c r="AI27" s="17">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>85</v>
       </c>
       <c r="AJ27" s="17">
-        <f t="shared" si="18"/>
+        <f t="shared" si="16"/>
         <v>175.48387770739737</v>
       </c>
     </row>
@@ -3574,7 +3574,7 @@
         <v>3965</v>
       </c>
       <c r="N28" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>4124.25</v>
       </c>
       <c r="O28" s="8">
@@ -3597,7 +3597,7 @@
         <v>3972.5714285714284</v>
       </c>
       <c r="U28" s="9">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>0.91708990172152238</v>
       </c>
       <c r="V28" s="5">
@@ -3609,7 +3609,7 @@
         <v>0.90576189740018953</v>
       </c>
       <c r="X28" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>5313.7142857142853</v>
       </c>
       <c r="Y28" s="9">
@@ -3617,11 +3617,11 @@
         <v>1.0788641703164428</v>
       </c>
       <c r="Z28" s="5">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>5658.5559495123453</v>
       </c>
       <c r="AA28" s="9">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>1.148878720497329</v>
       </c>
       <c r="AB28" s="5">
@@ -3639,11 +3639,11 @@
         <v>213</v>
       </c>
       <c r="AI28" s="17">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>61.571428571428442</v>
       </c>
       <c r="AJ28" s="17">
-        <f t="shared" si="18"/>
+        <f t="shared" si="16"/>
         <v>12.501750424077727</v>
       </c>
     </row>
@@ -3690,7 +3690,7 @@
         <v>4751</v>
       </c>
       <c r="N29" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>3860.25</v>
       </c>
       <c r="O29" s="8">
@@ -3713,7 +3713,7 @@
         <v>3918.7142857142858</v>
       </c>
       <c r="U29" s="9">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>0.92229843319211879</v>
       </c>
       <c r="V29" s="5">
@@ -3725,7 +3725,7 @@
         <v>0.90865213285330926</v>
       </c>
       <c r="X29" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>5595.2857142857147</v>
       </c>
       <c r="Y29" s="9">
@@ -3733,11 +3733,11 @@
         <v>1.0936836814475595</v>
       </c>
       <c r="Z29" s="5">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>5663.540542603223</v>
       </c>
       <c r="AA29" s="9">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>1.1070251256065722</v>
       </c>
       <c r="AB29" s="5">
@@ -3755,11 +3755,11 @@
         <v>509</v>
       </c>
       <c r="AI29" s="17">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>567.71428571428578</v>
       </c>
       <c r="AJ29" s="17">
-        <f t="shared" si="18"/>
+        <f t="shared" si="16"/>
         <v>509.73310504616074</v>
       </c>
     </row>
@@ -3806,7 +3806,7 @@
         <v>4615</v>
       </c>
       <c r="N30" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>3937.5</v>
       </c>
       <c r="O30" s="8">
@@ -3828,7 +3828,7 @@
         <v>3880</v>
       </c>
       <c r="U30" s="9">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>0.93026441978353192</v>
       </c>
       <c r="V30" s="14">
@@ -3840,7 +3840,7 @@
         <v>0.89906524637680563</v>
       </c>
       <c r="X30" s="14">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>5441.8571428571431</v>
       </c>
       <c r="Y30" s="9">
@@ -3848,11 +3848,11 @@
         <v>1.0291511320041067</v>
       </c>
       <c r="Z30" s="14">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>5654.516128385083</v>
       </c>
       <c r="AA30" s="18">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>1.0693686955934398</v>
       </c>
       <c r="AB30" s="14">
@@ -3868,11 +3868,11 @@
         <v>414</v>
       </c>
       <c r="AI30" s="17">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>471</v>
       </c>
       <c r="AJ30" s="17">
-        <f t="shared" si="18"/>
+        <f t="shared" si="16"/>
         <v>601.12729525468285</v>
       </c>
     </row>
@@ -3919,7 +3919,7 @@
         <v>5453</v>
       </c>
       <c r="N31" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>3805.5</v>
       </c>
       <c r="O31" s="8">
@@ -3941,7 +3941,7 @@
         <v>3826.1428571428573</v>
       </c>
       <c r="U31" s="9">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>0.94426032999576937</v>
       </c>
       <c r="V31" s="14">
@@ -3953,7 +3953,7 @@
         <v>0.91803142725764109</v>
       </c>
       <c r="X31" s="14">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>5330.2857142857147</v>
       </c>
       <c r="Y31" s="9">
@@ -3961,11 +3961,11 @@
         <v>0.99743370402053044</v>
       </c>
       <c r="Z31" s="14">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>5584.2720668052998</v>
       </c>
       <c r="AA31" s="18">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>1.044961090345303</v>
       </c>
       <c r="AB31" s="14">
@@ -3981,11 +3981,11 @@
         <v>196</v>
       </c>
       <c r="AI31" s="17">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>217.14285714285734</v>
       </c>
       <c r="AJ31" s="17">
-        <f t="shared" si="18"/>
+        <f t="shared" si="16"/>
         <v>110.86334324796189</v>
       </c>
     </row>
@@ -4032,7 +4032,7 @@
         <v>6156</v>
       </c>
       <c r="N32" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>3835.25</v>
       </c>
       <c r="O32" s="8">
@@ -4054,7 +4054,7 @@
         <v>3703.5714285714284</v>
       </c>
       <c r="U32" s="9">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>0.93228567318757194</v>
       </c>
       <c r="V32" s="14">
@@ -4066,7 +4066,7 @@
         <v>0.92905815763740374</v>
       </c>
       <c r="X32" s="14">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>5123.1428571428569</v>
       </c>
       <c r="Y32" s="9">
@@ -4074,11 +4074,11 @@
         <v>0.9641359285944725</v>
       </c>
       <c r="Z32" s="14">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>5954.461026581519</v>
       </c>
       <c r="AA32" s="18">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>1.1205835892588083</v>
       </c>
       <c r="AB32" s="14">
@@ -4094,11 +4094,11 @@
         <v>195</v>
       </c>
       <c r="AI32" s="17">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>326.42857142857156</v>
       </c>
       <c r="AJ32" s="17">
-        <f t="shared" si="18"/>
+        <f t="shared" si="16"/>
         <v>339.25010748843988</v>
       </c>
     </row>
@@ -4145,7 +4145,7 @@
         <v>6174</v>
       </c>
       <c r="N33" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>3940.25</v>
       </c>
       <c r="O33" s="8">
@@ -4167,7 +4167,7 @@
         <v>3616.5714285714284</v>
       </c>
       <c r="U33" s="9">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>0.92289745178812288</v>
       </c>
       <c r="V33" s="14">
@@ -4179,7 +4179,7 @@
         <v>0.94074193013997387</v>
       </c>
       <c r="X33" s="14">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>4954.2857142857147</v>
       </c>
       <c r="Y33" s="9">
@@ -4187,11 +4187,11 @@
         <v>0.88543927285725232</v>
       </c>
       <c r="Z33" s="14">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>5561.3835509154533</v>
       </c>
       <c r="AA33" s="18">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>0.99394094151730206</v>
       </c>
       <c r="AB33" s="14">
@@ -4207,11 +4207,11 @@
         <v>169</v>
       </c>
       <c r="AI33" s="17">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>154.42857142857156</v>
       </c>
       <c r="AJ33" s="17">
-        <f t="shared" si="18"/>
+        <f t="shared" si="16"/>
         <v>84.501159190053841</v>
       </c>
     </row>
@@ -4258,7 +4258,7 @@
         <v>6082</v>
       </c>
       <c r="N34" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>3792.5</v>
       </c>
       <c r="O34" s="8">
@@ -4283,7 +4283,7 @@
         <v>3472.7142857142858</v>
       </c>
       <c r="U34" s="9">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>0.89502945508100151</v>
       </c>
       <c r="V34" s="14">
@@ -4295,7 +4295,7 @@
         <v>0.94528742393781351</v>
       </c>
       <c r="X34" s="14">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>4832.7142857142853</v>
       </c>
       <c r="Y34" s="9">
@@ -4303,11 +4303,11 @@
         <v>0.88806342372614377</v>
       </c>
       <c r="Z34" s="14">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>5318.8875859677237</v>
       </c>
       <c r="AA34" s="18">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>0.97740301634877969</v>
       </c>
       <c r="AB34" s="14">
@@ -4339,11 +4339,11 @@
         <v>32</v>
       </c>
       <c r="AI34" s="17">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>287.28571428571422</v>
       </c>
       <c r="AJ34" s="17">
-        <f t="shared" si="18"/>
+        <f t="shared" si="16"/>
         <v>92.284795121283423</v>
       </c>
     </row>
@@ -4390,7 +4390,7 @@
         <v>5936</v>
       </c>
       <c r="N35" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>3653.5</v>
       </c>
       <c r="O35" s="8">
@@ -4415,7 +4415,7 @@
         <v>3400.5714285714284</v>
       </c>
       <c r="U35" s="9">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>0.88877272896986892</v>
       </c>
       <c r="V35" s="14">
@@ -4427,7 +4427,7 @@
         <v>0.91919790100732257</v>
       </c>
       <c r="X35" s="14">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>4554.2857142857147</v>
       </c>
       <c r="Y35" s="9">
@@ -4435,11 +4435,11 @@
         <v>0.85441680960548883</v>
       </c>
       <c r="Z35" s="14">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>4960.2874440459718</v>
       </c>
       <c r="AA35" s="18">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>0.93058565899232959</v>
       </c>
       <c r="AB35" s="14">
@@ -4471,11 +4471,11 @@
         <v>600</v>
       </c>
       <c r="AI35" s="17">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>347.57142857142844</v>
       </c>
       <c r="AJ35" s="17">
-        <f t="shared" si="18"/>
+        <f t="shared" si="16"/>
         <v>463.98248323987445</v>
       </c>
     </row>
@@ -4522,7 +4522,7 @@
         <v>3677</v>
       </c>
       <c r="N36" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>3331.5</v>
       </c>
       <c r="O36" s="8">
@@ -4547,7 +4547,7 @@
         <v>3239.7142857142858</v>
       </c>
       <c r="U36" s="9">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>0.87475409836065576</v>
       </c>
       <c r="V36" s="14">
@@ -4559,7 +4559,7 @@
         <v>0.91592208848937307</v>
       </c>
       <c r="X36" s="14">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>4109.2857142857147</v>
       </c>
       <c r="Y36" s="9">
@@ -4567,11 +4567,11 @@
         <v>0.8021025040432771</v>
       </c>
       <c r="Z36" s="14">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>4455.8685400286404</v>
       </c>
       <c r="AA36" s="18">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>0.86975293570354373</v>
       </c>
       <c r="AB36" s="14">
@@ -4603,11 +4603,11 @@
         <v>589</v>
       </c>
       <c r="AI36" s="17">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>497.71428571428578</v>
       </c>
       <c r="AJ36" s="17">
-        <f t="shared" si="18"/>
+        <f t="shared" si="16"/>
         <v>650.18287772671374</v>
       </c>
     </row>
@@ -4654,7 +4654,7 @@
         <v>3834</v>
       </c>
       <c r="N37" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>3224.75</v>
       </c>
       <c r="O37" s="8">
@@ -4679,7 +4679,7 @@
         <v>3090.2857142857142</v>
       </c>
       <c r="U37" s="9">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>0.85447938062885131</v>
       </c>
       <c r="V37" s="5">
@@ -4691,7 +4691,7 @@
         <v>0.88071788832862941</v>
       </c>
       <c r="X37" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>3946.4285714285716</v>
       </c>
       <c r="Y37" s="9">
@@ -4699,11 +4699,11 @@
         <v>0.79656862745098034</v>
       </c>
       <c r="Z37" s="5">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>4412.1178806516027</v>
       </c>
       <c r="AA37" s="26">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>0.89056589286508703</v>
       </c>
       <c r="AB37" s="5">
@@ -4735,11 +4735,11 @@
         <v>119</v>
       </c>
       <c r="AI37" s="17">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>253.71428571428578</v>
       </c>
       <c r="AJ37" s="17">
-        <f t="shared" si="18"/>
+        <f t="shared" si="16"/>
         <v>158.82084843891698</v>
       </c>
     </row>
@@ -4786,7 +4786,7 @@
         <v>4003</v>
       </c>
       <c r="N38" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>3060.75</v>
       </c>
       <c r="O38" s="8">
@@ -4811,7 +4811,7 @@
         <v>2886.5714285714284</v>
       </c>
       <c r="U38" s="9">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>0.83121477642025587</v>
       </c>
       <c r="V38" s="5">
@@ -4823,7 +4823,7 @@
         <v>0.89055250983081524</v>
       </c>
       <c r="X38" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>3696.1428571428573</v>
       </c>
       <c r="Y38" s="9">
@@ -4831,11 +4831,11 @@
         <v>0.76481716870141014</v>
       </c>
       <c r="Z38" s="5">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>4091.9303084650005</v>
       </c>
       <c r="AA38" s="9">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>0.8467147169368</v>
       </c>
       <c r="AB38" s="5">
@@ -4867,11 +4867,11 @@
         <v>43</v>
       </c>
       <c r="AI38" s="17">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>217.42857142857156</v>
       </c>
       <c r="AJ38" s="17">
-        <f t="shared" si="18"/>
+        <f t="shared" si="16"/>
         <v>11.365576931816122</v>
       </c>
     </row>
@@ -4918,7 +4918,7 @@
         <v>4974</v>
       </c>
       <c r="N39" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>3023.5</v>
       </c>
       <c r="O39" s="8">
@@ -4943,7 +4943,7 @@
         <v>2739.8571428571427</v>
       </c>
       <c r="U39" s="9">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>0.80570492354226175</v>
       </c>
       <c r="V39" s="5">
@@ -4955,7 +4955,7 @@
         <v>0.85986954065208154</v>
       </c>
       <c r="X39" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>3479.4285714285716</v>
       </c>
       <c r="Y39" s="9">
@@ -4963,11 +4963,11 @@
         <v>0.76398996235884564</v>
       </c>
       <c r="Z39" s="5">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>3582.6568256432533</v>
       </c>
       <c r="AA39" s="9">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>0.78665614113873183</v>
       </c>
       <c r="AB39" s="5">
@@ -4999,11 +4999,11 @@
         <v>119</v>
       </c>
       <c r="AI39" s="17">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>164.14285714285734</v>
       </c>
       <c r="AJ39" s="17">
-        <f t="shared" si="18"/>
+        <f t="shared" si="16"/>
         <v>20.04779224030699</v>
       </c>
     </row>
@@ -5050,7 +5050,7 @@
         <v>5323</v>
       </c>
       <c r="N40" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>3019.25</v>
       </c>
       <c r="O40" s="8">
@@ -5075,7 +5075,7 @@
         <v>2632.8571428571427</v>
       </c>
       <c r="U40" s="9">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>0.81268189434694404</v>
       </c>
       <c r="V40" s="5">
@@ -5087,7 +5087,7 @@
         <v>0.85250846830509663</v>
       </c>
       <c r="X40" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>3178.2857142857142</v>
       </c>
       <c r="Y40" s="9">
@@ -5095,11 +5095,11 @@
         <v>0.77343994437684682</v>
       </c>
       <c r="Z40" s="5">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>3345.4943069333103</v>
       </c>
       <c r="AA40" s="9">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>0.81413037192884308</v>
       </c>
       <c r="AB40" s="5">
@@ -5131,11 +5131,11 @@
         <v>294</v>
       </c>
       <c r="AI40" s="17">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>92.142857142857338</v>
       </c>
       <c r="AJ40" s="17">
-        <f t="shared" si="18"/>
+        <f t="shared" si="16"/>
         <v>36.8838634604258</v>
       </c>
     </row>
@@ -5182,7 +5182,7 @@
         <v>4133</v>
       </c>
       <c r="N41" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>2766.75</v>
       </c>
       <c r="O41" s="8">
@@ -5207,7 +5207,7 @@
         <v>2432.1428571428573</v>
       </c>
       <c r="U41" s="9">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>0.78702847633136097</v>
       </c>
       <c r="V41" s="5">
@@ -5219,7 +5219,7 @@
         <v>0.81730653150416632</v>
       </c>
       <c r="X41" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>2900.7142857142858</v>
       </c>
       <c r="Y41" s="9">
@@ -5227,11 +5227,11 @@
         <v>0.73502262443438915</v>
       </c>
       <c r="Z41" s="5">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>2931.0885490659284</v>
       </c>
       <c r="AA41" s="9">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>0.7427192703515475</v>
       </c>
       <c r="AB41" s="5">
@@ -5263,11 +5263,11 @@
         <v>433</v>
       </c>
       <c r="AI41" s="17">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>98.142857142857338</v>
       </c>
       <c r="AJ41" s="17">
-        <f t="shared" si="18"/>
+        <f t="shared" si="16"/>
         <v>191.71069849973219</v>
       </c>
     </row>
@@ -5314,7 +5314,7 @@
         <v>2821</v>
       </c>
       <c r="N42" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>2497.25</v>
       </c>
       <c r="O42" s="8">
@@ -5339,7 +5339,7 @@
         <v>2275.4285714285716</v>
       </c>
       <c r="U42" s="9">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>0.78828070870038613</v>
       </c>
       <c r="V42" s="5">
@@ -5351,7 +5351,7 @@
         <v>0.80599093417074463</v>
       </c>
       <c r="X42" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>2825.8571428571427</v>
       </c>
       <c r="Y42" s="9">
@@ -5359,11 +5359,11 @@
         <v>0.7645421868356973</v>
       </c>
       <c r="Z42" s="5">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>2704.9796601669432</v>
       </c>
       <c r="AA42" s="9">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>0.73183850427737795</v>
       </c>
       <c r="AB42" s="5">
@@ -5395,11 +5395,11 @@
         <v>471</v>
       </c>
       <c r="AI42" s="17">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>249.42857142857156</v>
       </c>
       <c r="AJ42" s="17">
-        <f t="shared" si="18"/>
+        <f t="shared" si="16"/>
         <v>300.55040226486653</v>
       </c>
     </row>
@@ -5446,7 +5446,7 @@
         <v>2537</v>
       </c>
       <c r="N43" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>2269.5</v>
       </c>
       <c r="O43" s="8">
@@ -5471,7 +5471,7 @@
         <v>2139.1428571428573</v>
       </c>
       <c r="U43" s="9">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>0.78074977840346227</v>
       </c>
       <c r="V43" s="5">
@@ -5483,7 +5483,7 @@
         <v>0.81251748820707959</v>
       </c>
       <c r="X43" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>2774</v>
       </c>
       <c r="Y43" s="9">
@@ -5491,11 +5491,11 @@
         <v>0.79725734931844305</v>
       </c>
       <c r="Z43" s="5">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>2543.1984407338614</v>
       </c>
       <c r="AA43" s="26">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>0.73092417002533372</v>
       </c>
       <c r="AB43" s="5">
@@ -5527,11 +5527,11 @@
         <v>276</v>
       </c>
       <c r="AI43" s="17">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>146.14285714285734</v>
       </c>
       <c r="AJ43" s="17">
-        <f t="shared" si="18"/>
+        <f t="shared" si="16"/>
         <v>233.18184376051113</v>
       </c>
     </row>
@@ -5578,7 +5578,7 @@
         <v>2082</v>
       </c>
       <c r="N44" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>2073</v>
       </c>
       <c r="O44" s="8">
@@ -5603,7 +5603,7 @@
         <v>2005.4285714285713</v>
       </c>
       <c r="U44" s="9">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>0.76169289202387414</v>
       </c>
       <c r="V44" s="14">
@@ -5615,7 +5615,7 @@
         <v>0.76153580023828582</v>
       </c>
       <c r="X44" s="14">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>2665.1428571428573</v>
       </c>
       <c r="Y44" s="9">
@@ -5623,11 +5623,11 @@
         <v>0.83854728514922694</v>
       </c>
       <c r="Z44" s="14">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>2335.9731480190112</v>
       </c>
       <c r="AA44" s="28">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>0.73497896602539903</v>
       </c>
       <c r="AB44" s="14">
@@ -5659,11 +5659,11 @@
         <v>134</v>
       </c>
       <c r="AI44" s="17">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>66.428571428571331</v>
       </c>
       <c r="AJ44" s="17">
-        <f t="shared" si="18"/>
+        <f t="shared" si="16"/>
         <v>66.014971198800822</v>
       </c>
     </row>
@@ -5710,7 +5710,7 @@
         <v>2486</v>
       </c>
       <c r="N45" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>1991.25</v>
       </c>
       <c r="O45" s="8">
@@ -5735,7 +5735,7 @@
         <v>1913.8571428571429</v>
       </c>
       <c r="U45" s="9">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>0.78690161527165925</v>
       </c>
       <c r="V45" s="14">
@@ -5747,7 +5747,7 @@
         <v>0.77628884768259199</v>
       </c>
       <c r="X45" s="14">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>2622.7142857142858</v>
       </c>
       <c r="Y45" s="9">
@@ -5755,11 +5755,11 @@
         <v>0.90416153656734799</v>
       </c>
       <c r="Z45" s="14">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>2427.396660399007</v>
       </c>
       <c r="AA45" s="18">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>0.83682721609421562</v>
       </c>
       <c r="AB45" s="14">
@@ -5791,11 +5791,11 @@
         <v>16</v>
       </c>
       <c r="AI45" s="17">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>93.14285714285711</v>
       </c>
       <c r="AJ45" s="17">
-        <f t="shared" si="18"/>
+        <f t="shared" si="16"/>
         <v>118.95462402912426</v>
       </c>
     </row>
@@ -5842,7 +5842,7 @@
         <v>2866</v>
       </c>
       <c r="N46" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>1972.25</v>
       </c>
       <c r="O46" s="8">
@@ -5867,7 +5867,7 @@
         <v>1834.8571428571429</v>
       </c>
       <c r="U46" s="9">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>0.80637870416875934</v>
       </c>
       <c r="V46" s="14">
@@ -5879,7 +5879,7 @@
         <v>0.78374385879855979</v>
       </c>
       <c r="X46" s="14">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>2587.1428571428573</v>
       </c>
       <c r="Y46" s="9">
@@ -5887,11 +5887,11 @@
         <v>0.91552499873616111</v>
       </c>
       <c r="Z46" s="14">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>2441.7527721241904</v>
       </c>
       <c r="AA46" s="18">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>0.8640750925064119</v>
       </c>
       <c r="AB46" s="14">
@@ -5923,11 +5923,11 @@
         <v>22</v>
       </c>
       <c r="AI46" s="17">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>115.14285714285711</v>
       </c>
       <c r="AJ46" s="17">
-        <f t="shared" si="18"/>
+        <f t="shared" si="16"/>
         <v>166.64683100807702</v>
       </c>
     </row>
@@ -5974,7 +5974,7 @@
         <v>3380</v>
       </c>
       <c r="N47" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>1921.25</v>
       </c>
       <c r="O47" s="8">
@@ -5999,7 +5999,7 @@
         <v>1740.5714285714287</v>
       </c>
       <c r="U47" s="9">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>0.81367704020301856</v>
       </c>
       <c r="V47" s="14">
@@ -6011,7 +6011,7 @@
         <v>0.77670789566859344</v>
       </c>
       <c r="X47" s="14">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>2513.7142857142858</v>
       </c>
       <c r="Y47" s="9">
@@ -6019,11 +6019,11 @@
         <v>0.90616953342259765</v>
       </c>
       <c r="Z47" s="14">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>2383.507783802509</v>
       </c>
       <c r="AA47" s="18">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>0.85923135681417051</v>
       </c>
       <c r="AB47" s="14">
@@ -6055,11 +6055,11 @@
         <v>132</v>
       </c>
       <c r="AI47" s="17">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>48.428571428571331</v>
       </c>
       <c r="AJ47" s="17">
-        <f t="shared" si="18"/>
+        <f t="shared" si="16"/>
         <v>127.51085289406865</v>
       </c>
     </row>
@@ -6106,7 +6106,7 @@
         <v>3609</v>
       </c>
       <c r="N48" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>1859.75</v>
       </c>
       <c r="O48" s="8">
@@ -6131,7 +6131,7 @@
         <v>1688.2857142857142</v>
       </c>
       <c r="U48" s="9">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>0.84185781450349051</v>
       </c>
       <c r="V48" s="14">
@@ -6143,7 +6143,7 @@
         <v>0.80895208532992613</v>
       </c>
       <c r="X48" s="14">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>2364.7142857142858</v>
       </c>
       <c r="Y48" s="9">
@@ -6151,11 +6151,11 @@
         <v>0.88727487135506</v>
       </c>
       <c r="Z48" s="14">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>2421.0799315037029</v>
       </c>
       <c r="AA48" s="28">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>0.90842407378462264</v>
       </c>
       <c r="AB48" s="14">
@@ -6187,11 +6187,11 @@
         <v>167</v>
       </c>
       <c r="AI48" s="17">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>4.7142857142857792</v>
       </c>
       <c r="AJ48" s="17">
-        <f t="shared" si="18"/>
+        <f t="shared" si="16"/>
         <v>70.704375162642464</v>
       </c>
     </row>
@@ -6238,7 +6238,7 @@
         <v>2458</v>
       </c>
       <c r="N49" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>1726.25</v>
       </c>
       <c r="O49" s="8">
@@ -6263,7 +6263,7 @@
         <v>1599.4285714285713</v>
       </c>
       <c r="U49" s="9">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>0.83570948719862648</v>
       </c>
       <c r="V49" s="14">
@@ -6275,7 +6275,7 @@
         <v>0.81960682103495752</v>
       </c>
       <c r="X49" s="14">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>2142.7142857142858</v>
       </c>
       <c r="Y49" s="9">
@@ -6283,11 +6283,11 @@
         <v>0.81698349583310637</v>
       </c>
       <c r="Z49" s="14">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>2385.6582777866156</v>
       </c>
       <c r="AA49" s="18">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>0.90961424611941333</v>
       </c>
       <c r="AB49" s="14">
@@ -6319,11 +6319,11 @@
         <v>253</v>
       </c>
       <c r="AI49" s="17">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>126.42857142857133</v>
       </c>
       <c r="AJ49" s="17">
-        <f t="shared" si="18"/>
+        <f t="shared" si="16"/>
         <v>95.610368772189531</v>
       </c>
     </row>
@@ -6370,7 +6370,7 @@
         <v>1775</v>
       </c>
       <c r="N50" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>1572</v>
       </c>
       <c r="O50" s="8">
@@ -6395,7 +6395,7 @@
         <v>1511</v>
       </c>
       <c r="U50" s="9">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>0.82349735284957959</v>
       </c>
       <c r="V50" s="14">
@@ -6407,7 +6407,7 @@
         <v>0.80956586584197299</v>
       </c>
       <c r="X50" s="14">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>2039.7142857142858</v>
       </c>
       <c r="Y50" s="9">
@@ -6415,11 +6415,11 @@
         <v>0.78840419657647709</v>
       </c>
       <c r="Z50" s="14">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>2299.9704746974303</v>
       </c>
       <c r="AA50" s="18">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>0.88900018348326948</v>
       </c>
       <c r="AB50" s="14">
@@ -6451,11 +6451,11 @@
         <v>239</v>
       </c>
       <c r="AI50" s="17">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>178</v>
       </c>
       <c r="AJ50" s="17">
-        <f t="shared" si="18"/>
+        <f t="shared" si="16"/>
         <v>152.43771155347167</v>
       </c>
     </row>
@@ -6502,7 +6502,7 @@
         <v>1785</v>
       </c>
       <c r="N51" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>1518</v>
       </c>
       <c r="O51" s="8">
@@ -6527,7 +6527,7 @@
         <v>1442.5714285714287</v>
       </c>
       <c r="U51" s="9">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>0.82879185817465528</v>
       </c>
       <c r="V51" s="5">
@@ -6539,7 +6539,7 @@
         <v>0.84729270427305181</v>
       </c>
       <c r="X51" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>1931.5714285714287</v>
       </c>
       <c r="Y51" s="9">
@@ -6547,11 +6547,11 @@
         <v>0.76841327574448737</v>
       </c>
       <c r="Z51" s="5">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>2153.1496801278086</v>
       </c>
       <c r="AA51" s="26">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>0.8565610230106081</v>
       </c>
       <c r="AB51" s="5">
@@ -6634,7 +6634,7 @@
         <v>2237</v>
       </c>
       <c r="N52" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>1441</v>
       </c>
       <c r="O52" s="8">
@@ -6659,7 +6659,7 @@
         <v>1370.7142857142858</v>
       </c>
       <c r="U52" s="9">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>0.81189710610932486</v>
       </c>
       <c r="V52" s="5">
@@ -6671,7 +6671,7 @@
         <v>0.82347794116312945</v>
       </c>
       <c r="X52" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>1840</v>
       </c>
       <c r="Y52" s="9">
@@ -6679,11 +6679,11 @@
         <v>0.77810668760949675</v>
       </c>
       <c r="Z52" s="5">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>1886.5696439251556</v>
       </c>
       <c r="AA52" s="9">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>0.79780024814088613</v>
       </c>
       <c r="AB52" s="5">
@@ -6766,7 +6766,7 @@
         <v>2352</v>
       </c>
       <c r="N53" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>1405.5</v>
       </c>
       <c r="O53" s="8">
@@ -6791,7 +6791,7 @@
         <v>1307.4285714285713</v>
       </c>
       <c r="U53" s="9">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>0.81743479814219366</v>
       </c>
       <c r="V53" s="5">
@@ -6803,7 +6803,7 @@
         <v>0.81720098455985113</v>
       </c>
       <c r="X53" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>1706.7142857142858</v>
       </c>
       <c r="Y53" s="9">
@@ -6811,11 +6811,11 @@
         <v>0.79651976798453228</v>
       </c>
       <c r="Z53" s="5">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>1757.8521611595409</v>
       </c>
       <c r="AA53" s="9">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>0.82038570092118046</v>
       </c>
       <c r="AB53" s="5">
@@ -6898,7 +6898,7 @@
         <v>2337</v>
       </c>
       <c r="N54" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>1399.75</v>
       </c>
       <c r="O54" s="8">
@@ -6923,7 +6923,7 @@
         <v>1251.4285714285713</v>
       </c>
       <c r="U54" s="9">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>0.82821215845702933</v>
       </c>
       <c r="V54" s="5">
@@ -6935,7 +6935,7 @@
         <v>0.83557581148706905</v>
       </c>
       <c r="X54" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>1581.8571428571429</v>
       </c>
       <c r="Y54" s="9">
@@ -6943,11 +6943,11 @@
         <v>0.77552878554419391</v>
       </c>
       <c r="Z54" s="5">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>1595.2553146569589</v>
       </c>
       <c r="AA54" s="9">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>0.78209743679778065</v>
       </c>
       <c r="AB54" s="5">
@@ -7030,7 +7030,7 @@
         <v>2055</v>
       </c>
       <c r="N55" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>1304</v>
       </c>
       <c r="O55" s="8">
@@ -7055,7 +7055,7 @@
         <v>1188.1428571428571</v>
       </c>
       <c r="U55" s="9">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>0.82362844127550006</v>
       </c>
       <c r="V55" s="5">
@@ -7067,7 +7067,7 @@
         <v>0.81767645224086472</v>
       </c>
       <c r="X55" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>1482.1428571428571</v>
       </c>
       <c r="Y55" s="9">
@@ -7075,11 +7075,11 @@
         <v>0.7673249020042896</v>
       </c>
       <c r="Z55" s="5">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>1488.3985117467357</v>
       </c>
       <c r="AA55" s="9">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>0.7705635368853746</v>
       </c>
       <c r="AB55" s="5">
@@ -7162,7 +7162,7 @@
         <v>1737</v>
       </c>
       <c r="N56" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>1215.25</v>
       </c>
       <c r="O56" s="8">
@@ -7187,7 +7187,7 @@
         <v>1125.1428571428571</v>
       </c>
       <c r="U56" s="9">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>0.82084418968212602</v>
       </c>
       <c r="V56" s="5">
@@ -7199,7 +7199,7 @@
         <v>0.82089061564387356</v>
       </c>
       <c r="X56" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>1323.5714285714287</v>
       </c>
       <c r="Y56" s="9">
@@ -7207,11 +7207,11 @@
         <v>0.71933229813664601</v>
       </c>
       <c r="Z56" s="5">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>1390.2994477917587</v>
       </c>
       <c r="AA56" s="9">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>0.75559752597378194</v>
       </c>
       <c r="AB56" s="5">
@@ -7294,7 +7294,7 @@
         <v>1018</v>
       </c>
       <c r="N57" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>1117.75</v>
       </c>
       <c r="O57" s="8">
@@ -7319,7 +7319,7 @@
         <v>1065.1428571428571</v>
       </c>
       <c r="U57" s="9">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>0.81468531468531469</v>
       </c>
       <c r="V57" s="5">
@@ -7331,7 +7331,7 @@
         <v>0.82549445988055636</v>
       </c>
       <c r="X57" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>1188.7142857142858</v>
       </c>
       <c r="Y57" s="9">
@@ -7339,11 +7339,11 @@
         <v>0.69649284339164641</v>
       </c>
       <c r="Z57" s="5">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>1267.447314964533</v>
       </c>
       <c r="AA57" s="26">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>0.74262419057099949</v>
       </c>
       <c r="AB57" s="5">
@@ -7426,7 +7426,7 @@
         <v>1144</v>
       </c>
       <c r="N58" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>1072.75</v>
       </c>
       <c r="O58" s="8">
@@ -7451,7 +7451,7 @@
         <v>1008.4285714285714</v>
       </c>
       <c r="U58" s="9">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>0.80582191780821921</v>
       </c>
       <c r="V58" s="14">
@@ -7463,7 +7463,7 @@
         <v>0.81710513708744226</v>
       </c>
       <c r="X58" s="14">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>1140.2857142857142</v>
       </c>
       <c r="Y58" s="9">
@@ -7471,11 +7471,11 @@
         <v>0.72085252415786139</v>
       </c>
       <c r="Z58" s="14">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>1227.2756757755546</v>
       </c>
       <c r="AA58" s="18">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>0.77584482348314665</v>
       </c>
       <c r="AB58" s="45"/>
@@ -7552,7 +7552,7 @@
         <v>1304</v>
       </c>
       <c r="N59" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>1011.25</v>
       </c>
       <c r="O59" s="8">
@@ -7577,7 +7577,7 @@
         <v>946.28571428571433</v>
       </c>
       <c r="U59" s="9">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>0.79644102440783948</v>
       </c>
       <c r="V59" s="14">
@@ -7589,7 +7589,7 @@
         <v>0.81241640640341151</v>
       </c>
       <c r="X59" s="14">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>1074.7142857142858</v>
       </c>
       <c r="Y59" s="9">
@@ -7597,11 +7597,11 @@
         <v>0.72510843373493983</v>
       </c>
       <c r="Z59" s="14">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>1079.5264514321748</v>
       </c>
       <c r="AA59" s="18">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>0.7283551961470095</v>
       </c>
       <c r="AB59" s="45"/>
@@ -7678,7 +7678,7 @@
         <v>1478</v>
       </c>
       <c r="N60" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>981.5</v>
       </c>
       <c r="O60" s="8">
@@ -7703,7 +7703,7 @@
         <v>905.85714285714289</v>
       </c>
       <c r="U60" s="9">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>0.80510411376333169</v>
       </c>
       <c r="V60" s="14">
@@ -7715,7 +7715,7 @@
         <v>0.81158952992588029</v>
       </c>
       <c r="X60" s="14">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>1023.7142857142857</v>
       </c>
       <c r="Y60" s="9">
@@ -7723,11 +7723,11 @@
         <v>0.77344846195358863</v>
       </c>
       <c r="Z60" s="14">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>956.498116347571</v>
       </c>
       <c r="AA60" s="28">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>0.72266452395391223</v>
       </c>
       <c r="AB60" s="47"/>
@@ -7804,7 +7804,7 @@
         <v>1639</v>
       </c>
       <c r="N61" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>974.5</v>
       </c>
       <c r="O61" s="8">
@@ -7829,7 +7829,7 @@
         <v>890.28571428571433</v>
       </c>
       <c r="U61" s="9">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>0.8358369098712447</v>
       </c>
       <c r="V61" s="14">
@@ -7841,7 +7841,7 @@
         <v>0.81336120003637358</v>
       </c>
       <c r="X61" s="14">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>996</v>
       </c>
       <c r="Y61" s="9">
@@ -7849,11 +7849,11 @@
         <v>0.83788006249248881</v>
       </c>
       <c r="Z61" s="14">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>895.71714049397906</v>
       </c>
       <c r="AA61" s="18">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>0.7535176040689644</v>
       </c>
       <c r="AB61" s="47"/>
@@ -7930,7 +7930,7 @@
         <v>945</v>
       </c>
       <c r="N62" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>880.75</v>
       </c>
       <c r="O62" s="8">
@@ -7955,7 +7955,7 @@
         <v>869.14285714285711</v>
       </c>
       <c r="U62" s="9">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>0.86187845303867394</v>
       </c>
       <c r="V62" s="14">
@@ -7967,7 +7967,7 @@
         <v>0.79404890114078697</v>
       </c>
       <c r="X62" s="14">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>934.57142857142856</v>
       </c>
       <c r="Y62" s="9">
@@ -7975,11 +7975,11 @@
         <v>0.81959408669506395</v>
       </c>
       <c r="Z62" s="14">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>802.99794604239116</v>
       </c>
       <c r="AA62" s="18">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>0.70420767004469287</v>
       </c>
       <c r="AB62" s="47"/>
@@ -8056,7 +8056,7 @@
         <v>793</v>
       </c>
       <c r="N63" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>831.5</v>
       </c>
       <c r="O63" s="8">
@@ -8081,7 +8081,7 @@
         <v>877.57142857142856</v>
       </c>
       <c r="U63" s="9">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>0.92738526570048307</v>
       </c>
       <c r="V63" s="14">
@@ -8093,7 +8093,7 @@
         <v>0.81357768144547926</v>
       </c>
       <c r="X63" s="14">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>978.28571428571433</v>
       </c>
       <c r="Y63" s="9">
@@ -8101,11 +8101,11 @@
         <v>0.91027515618769106</v>
       </c>
       <c r="Z63" s="14">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>813.59480015988754</v>
       </c>
       <c r="AA63" s="28">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>0.75703357717921205</v>
       </c>
       <c r="AB63" s="47"/>
@@ -8182,7 +8182,7 @@
         <v>679</v>
       </c>
       <c r="N64" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>811.75</v>
       </c>
       <c r="O64" s="8">
@@ -8207,7 +8207,7 @@
         <v>881.14285714285711</v>
       </c>
       <c r="U64" s="9">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>0.9727172370288597</v>
       </c>
       <c r="V64" s="5">
@@ -8227,11 +8227,11 @@
         <v>0.93804074797655601</v>
       </c>
       <c r="Z64" s="5">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>867.56980433131753</v>
       </c>
       <c r="AA64" s="9">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>0.84747259703031297</v>
       </c>
       <c r="AB64" s="47"/>
@@ -8308,7 +8308,7 @@
         <v>685</v>
       </c>
       <c r="N65" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>829</v>
       </c>
       <c r="O65" s="8">
@@ -8341,11 +8341,11 @@
       <c r="X65" s="41"/>
       <c r="Y65" s="42"/>
       <c r="Z65" s="5">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>833.05362718736194</v>
       </c>
       <c r="AA65" s="9">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>0.83639922408369671</v>
       </c>
       <c r="AB65" s="47"/>
@@ -8410,7 +8410,7 @@
         <v>947</v>
       </c>
       <c r="N66" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>891</v>
       </c>
       <c r="O66" s="8">
@@ -8443,11 +8443,11 @@
       <c r="X66" s="41"/>
       <c r="Y66" s="42"/>
       <c r="Z66" s="5">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>931.54209218330277</v>
       </c>
       <c r="AA66" s="9">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>0.99675858228112502</v>
       </c>
       <c r="AB66" s="47"/>
@@ -8512,7 +8512,7 @@
         <v>1284</v>
       </c>
       <c r="N67" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>938.25</v>
       </c>
       <c r="O67" s="8">
@@ -8535,7 +8535,7 @@
       <c r="T67" s="41"/>
       <c r="U67" s="42"/>
       <c r="V67" s="5">
-        <f t="shared" si="26"/>
+        <f>AVERAGE(D64:D67,U64^1.75*D61,U64^1.75*D62,U64^1.75*D63)</f>
         <v>864.8398007603879</v>
       </c>
       <c r="W67" s="9">
@@ -9480,8 +9480,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:D54"/>
   <sheetViews>
-    <sheetView topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="B52" sqref="B52"/>
+    <sheetView topLeftCell="B23" workbookViewId="0">
+      <selection activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>